<commit_message>
Variable for harmonizing legumes was missing in DD. The variable DV491 is AV491 in S1_P1
</commit_message>
<xml_diff>
--- a/rmonize/data_dictionary/DD_KORA_S3_P1.xlsx
+++ b/rmonize/data_dictionary/DD_KORA_S3_P1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28224"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\NFDI4Health\TA5\Pilotprojekte\Pilotprojekt UC5.1\Study-specific DDs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="8_{E5BE394D-E05C-4703-BB6C-52AECCF72314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AC070B0D-E35C-43EA-908A-6154DCCF3C9C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CE3F2DF-4FEF-4D5B-A162-C2E4A38B5C36}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{1200B70D-B446-4CDA-99A8-3FD394D791D2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{1200B70D-B446-4CDA-99A8-3FD394D791D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -21,23 +21,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="222">
   <si>
     <t>index</t>
   </si>
@@ -697,13 +686,19 @@
   </si>
   <si>
     <t>unknown</t>
+  </si>
+  <si>
+    <t>dry legumes</t>
+  </si>
+  <si>
+    <t>DV491</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -791,7 +786,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1103,13 +1098,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08A73012-5CAD-43B9-A281-79101DF4E1E0}">
-  <dimension ref="A1:F100"/>
+  <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="C103" sqref="C103"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="9"/>
     <col min="2" max="2" width="26.7109375" style="9" bestFit="1" customWidth="1"/>
@@ -1117,7 +1112,7 @@
     <col min="4" max="4" width="11.5703125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1131,7 +1126,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
         <v>1</v>
       </c>
@@ -1145,7 +1140,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <v>2</v>
       </c>
@@ -1159,7 +1154,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>3</v>
       </c>
@@ -1173,7 +1168,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>4</v>
       </c>
@@ -1187,7 +1182,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>5</v>
       </c>
@@ -1201,7 +1196,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>6</v>
       </c>
@@ -1215,7 +1210,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>7</v>
       </c>
@@ -1229,7 +1224,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>8</v>
       </c>
@@ -1243,7 +1238,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>9</v>
       </c>
@@ -1257,7 +1252,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>10</v>
       </c>
@@ -1271,7 +1266,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>11</v>
       </c>
@@ -1285,7 +1280,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>12</v>
       </c>
@@ -1299,7 +1294,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>13</v>
       </c>
@@ -1313,7 +1308,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>14</v>
       </c>
@@ -1327,7 +1322,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>15</v>
       </c>
@@ -1341,7 +1336,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>16</v>
       </c>
@@ -1355,7 +1350,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>17</v>
       </c>
@@ -1369,7 +1364,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
         <v>18</v>
       </c>
@@ -1383,7 +1378,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
         <v>19</v>
       </c>
@@ -1397,7 +1392,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
         <v>20</v>
       </c>
@@ -1411,7 +1406,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
         <v>21</v>
       </c>
@@ -1425,7 +1420,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
         <v>22</v>
       </c>
@@ -1439,7 +1434,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
         <v>23</v>
       </c>
@@ -1453,7 +1448,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
         <v>24</v>
       </c>
@@ -1467,7 +1462,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="9">
         <v>25</v>
       </c>
@@ -1481,7 +1476,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="9">
         <v>26</v>
       </c>
@@ -1495,7 +1490,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="9">
         <v>27</v>
       </c>
@@ -1509,7 +1504,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="9">
         <v>28</v>
       </c>
@@ -1523,7 +1518,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="9">
         <v>29</v>
       </c>
@@ -1537,7 +1532,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="9">
         <v>30</v>
       </c>
@@ -1551,7 +1546,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="9">
         <v>31</v>
       </c>
@@ -1565,7 +1560,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="9">
         <v>32</v>
       </c>
@@ -1579,7 +1574,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="9">
         <v>33</v>
       </c>
@@ -1593,7 +1588,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="9">
         <v>34</v>
       </c>
@@ -1607,7 +1602,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="9">
         <v>35</v>
       </c>
@@ -1621,7 +1616,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="9">
         <v>36</v>
       </c>
@@ -1635,7 +1630,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="9">
         <v>37</v>
       </c>
@@ -1649,7 +1644,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="9">
         <v>38</v>
       </c>
@@ -1663,7 +1658,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="9">
         <v>39</v>
       </c>
@@ -1677,7 +1672,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="9">
         <v>40</v>
       </c>
@@ -1691,7 +1686,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="9">
         <v>41</v>
       </c>
@@ -1705,7 +1700,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="9">
         <v>42</v>
       </c>
@@ -1719,7 +1714,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="9">
         <v>43</v>
       </c>
@@ -1733,7 +1728,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="9">
         <v>44</v>
       </c>
@@ -1747,7 +1742,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="9">
         <v>45</v>
       </c>
@@ -1761,7 +1756,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="9">
         <v>46</v>
       </c>
@@ -1775,7 +1770,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="9">
         <v>47</v>
       </c>
@@ -1789,7 +1784,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="9">
         <v>48</v>
       </c>
@@ -1803,7 +1798,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="9">
         <v>49</v>
       </c>
@@ -1817,7 +1812,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="9">
         <v>50</v>
       </c>
@@ -1831,7 +1826,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="9">
         <v>51</v>
       </c>
@@ -1845,7 +1840,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="9">
         <v>52</v>
       </c>
@@ -1859,7 +1854,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="9">
         <v>53</v>
       </c>
@@ -1873,7 +1868,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="9">
         <v>54</v>
       </c>
@@ -1887,7 +1882,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="9">
         <v>55</v>
       </c>
@@ -1901,7 +1896,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="9">
         <v>56</v>
       </c>
@@ -1915,7 +1910,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="9">
         <v>57</v>
       </c>
@@ -1929,7 +1924,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="9">
         <v>58</v>
       </c>
@@ -1943,7 +1938,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="9">
         <v>59</v>
       </c>
@@ -1957,7 +1952,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="9">
         <v>60</v>
       </c>
@@ -1971,7 +1966,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="9">
         <v>61</v>
       </c>
@@ -1985,7 +1980,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="9">
         <v>62</v>
       </c>
@@ -1999,7 +1994,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="9">
         <v>63</v>
       </c>
@@ -2013,7 +2008,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="9">
         <v>64</v>
       </c>
@@ -2027,7 +2022,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="9">
         <v>65</v>
       </c>
@@ -2041,7 +2036,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="9">
         <v>66</v>
       </c>
@@ -2055,7 +2050,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="9">
         <v>67</v>
       </c>
@@ -2069,7 +2064,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="9">
         <v>68</v>
       </c>
@@ -2083,7 +2078,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="9">
         <v>69</v>
       </c>
@@ -2097,7 +2092,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="9">
         <v>70</v>
       </c>
@@ -2111,7 +2106,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="9">
         <v>71</v>
       </c>
@@ -2125,7 +2120,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="73" spans="1:4">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="9">
         <v>72</v>
       </c>
@@ -2139,7 +2134,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="1:4">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="9">
         <v>73</v>
       </c>
@@ -2153,7 +2148,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="75" spans="1:4">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="9">
         <v>74</v>
       </c>
@@ -2167,7 +2162,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="76" spans="1:4">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="9">
         <v>75</v>
       </c>
@@ -2181,7 +2176,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="77" spans="1:4">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="9">
         <v>76</v>
       </c>
@@ -2195,7 +2190,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="78" spans="1:4">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="9">
         <v>77</v>
       </c>
@@ -2209,7 +2204,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="79" spans="1:4">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="9">
         <v>78</v>
       </c>
@@ -2223,7 +2218,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="80" spans="1:4">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="9">
         <v>79</v>
       </c>
@@ -2237,7 +2232,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="9">
         <v>80</v>
       </c>
@@ -2251,7 +2246,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="82" spans="1:6">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="9">
         <v>81</v>
       </c>
@@ -2265,7 +2260,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="83" spans="1:6">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="9">
         <v>82</v>
       </c>
@@ -2279,7 +2274,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="84" spans="1:6">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="9">
         <v>83</v>
       </c>
@@ -2293,7 +2288,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="85" spans="1:6">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="9">
         <v>84</v>
       </c>
@@ -2307,7 +2302,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="86" spans="1:6">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="9">
         <v>85</v>
       </c>
@@ -2321,7 +2316,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="9">
         <v>86</v>
       </c>
@@ -2335,7 +2330,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="88" spans="1:6">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="9">
         <v>87</v>
       </c>
@@ -2349,7 +2344,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="89" spans="1:6">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="9">
         <v>88</v>
       </c>
@@ -2363,7 +2358,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="90" spans="1:6">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="9">
         <v>89</v>
       </c>
@@ -2377,7 +2372,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="91" spans="1:6">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="9">
         <v>90</v>
       </c>
@@ -2394,7 +2389,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="92" spans="1:6">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="9">
         <v>91</v>
       </c>
@@ -2408,7 +2403,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="93" spans="1:6">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="9">
         <v>92</v>
       </c>
@@ -2422,7 +2417,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="94" spans="1:6">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="9">
         <v>93</v>
       </c>
@@ -2436,7 +2431,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="95" spans="1:6">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="9">
         <v>94</v>
       </c>
@@ -2450,7 +2445,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:6">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="9">
         <v>95</v>
       </c>
@@ -2464,7 +2459,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="97" spans="1:4">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="9">
         <v>96</v>
       </c>
@@ -2478,7 +2473,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="98" spans="1:4">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="9">
         <v>97</v>
       </c>
@@ -2492,7 +2487,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="99" spans="1:4">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="9">
         <v>98</v>
       </c>
@@ -2506,7 +2501,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="100" spans="1:4">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="9">
         <v>99</v>
       </c>
@@ -2517,6 +2512,20 @@
         <v>205</v>
       </c>
       <c r="D100" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="9">
+        <v>100</v>
+      </c>
+      <c r="B101" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="C101" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="D101" s="9" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2530,18 +2539,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7CFBFAA-22DC-428C-A718-7E0BADD40216}">
   <dimension ref="A1:E253"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>206</v>
       </c>
@@ -2556,7 +2565,7 @@
       </c>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" s="8" customFormat="1">
+    <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>7</v>
       </c>
@@ -2567,7 +2576,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="8" customFormat="1">
+    <row r="3" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>7</v>
       </c>
@@ -2578,7 +2587,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="8" customFormat="1">
+    <row r="4" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>12</v>
       </c>
@@ -2589,7 +2598,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="8" customFormat="1">
+    <row r="5" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>12</v>
       </c>
@@ -2600,7 +2609,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="8" customFormat="1">
+    <row r="6" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>12</v>
       </c>
@@ -2611,7 +2620,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="8" customFormat="1">
+    <row r="7" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>12</v>
       </c>
@@ -2622,7 +2631,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="8" customFormat="1">
+    <row r="8" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>12</v>
       </c>
@@ -2633,7 +2642,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="8" customFormat="1">
+    <row r="9" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>12</v>
       </c>
@@ -2644,7 +2653,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="8" customFormat="1">
+    <row r="10" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>14</v>
       </c>
@@ -2655,7 +2664,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="8" customFormat="1">
+    <row r="11" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>14</v>
       </c>
@@ -2666,7 +2675,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="8" customFormat="1">
+    <row r="12" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>14</v>
       </c>
@@ -2677,7 +2686,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="8" customFormat="1">
+    <row r="13" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>14</v>
       </c>
@@ -2688,1249 +2697,1249 @@
         <v>219</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="4"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="4"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="4"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="4"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="4"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="4"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="4"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="4"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="4"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="4"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="4"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="4"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="4"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="4"/>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="4"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="4"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="4"/>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="4"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="4"/>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="4"/>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="4"/>
       <c r="C34" s="8"/>
       <c r="D34" s="8"/>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="4"/>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="4"/>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="4"/>
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="4"/>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="4"/>
       <c r="C39" s="8"/>
       <c r="D39" s="8"/>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="4"/>
       <c r="C40" s="8"/>
       <c r="D40" s="8"/>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="4"/>
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="4"/>
       <c r="C42" s="8"/>
       <c r="D42" s="8"/>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
       <c r="B43" s="4"/>
       <c r="C43" s="8"/>
       <c r="D43" s="8"/>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
       <c r="B44" s="4"/>
       <c r="C44" s="8"/>
       <c r="D44" s="8"/>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
       <c r="B45" s="4"/>
       <c r="C45" s="8"/>
       <c r="D45" s="8"/>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
       <c r="B46" s="4"/>
       <c r="C46" s="8"/>
       <c r="D46" s="8"/>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
       <c r="B47" s="4"/>
       <c r="C47" s="8"/>
       <c r="D47" s="8"/>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" s="4"/>
       <c r="C48" s="8"/>
       <c r="D48" s="8"/>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
       <c r="B49" s="4"/>
       <c r="C49" s="8"/>
       <c r="D49" s="8"/>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
       <c r="B50" s="4"/>
       <c r="C50" s="8"/>
       <c r="D50" s="8"/>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
       <c r="B51" s="4"/>
       <c r="C51" s="8"/>
       <c r="D51" s="8"/>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
       <c r="B52" s="4"/>
       <c r="C52" s="8"/>
       <c r="D52" s="8"/>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="3"/>
       <c r="B53" s="4"/>
       <c r="C53" s="8"/>
       <c r="D53" s="8"/>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
       <c r="B54" s="4"/>
       <c r="C54" s="8"/>
       <c r="D54" s="8"/>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="3"/>
       <c r="B55" s="4"/>
       <c r="C55" s="8"/>
       <c r="D55" s="8"/>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
       <c r="B56" s="4"/>
       <c r="C56" s="8"/>
       <c r="D56" s="8"/>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="3"/>
       <c r="B57" s="4"/>
       <c r="C57" s="8"/>
       <c r="D57" s="8"/>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="3"/>
       <c r="B58" s="4"/>
       <c r="C58" s="8"/>
       <c r="D58" s="8"/>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="3"/>
       <c r="B59" s="4"/>
       <c r="C59" s="8"/>
       <c r="D59" s="8"/>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="3"/>
       <c r="B60" s="4"/>
       <c r="C60" s="8"/>
       <c r="D60" s="8"/>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="3"/>
       <c r="B61" s="4"/>
       <c r="C61" s="8"/>
       <c r="D61" s="8"/>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
       <c r="B62" s="4"/>
       <c r="C62" s="8"/>
       <c r="D62" s="8"/>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="3"/>
       <c r="B63" s="4"/>
       <c r="C63" s="8"/>
       <c r="D63" s="8"/>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="3"/>
       <c r="B64" s="4"/>
       <c r="C64" s="8"/>
       <c r="D64" s="8"/>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="3"/>
       <c r="B65" s="4"/>
       <c r="C65" s="8"/>
       <c r="D65" s="8"/>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="3"/>
       <c r="B66" s="4"/>
       <c r="C66" s="8"/>
       <c r="D66" s="8"/>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="3"/>
       <c r="B67" s="4"/>
       <c r="C67" s="8"/>
       <c r="D67" s="8"/>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
       <c r="B68" s="4"/>
       <c r="C68" s="8"/>
       <c r="D68" s="8"/>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="3"/>
       <c r="B69" s="4"/>
       <c r="C69" s="8"/>
       <c r="D69" s="8"/>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="3"/>
       <c r="B70" s="4"/>
       <c r="C70" s="8"/>
       <c r="D70" s="8"/>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="3"/>
       <c r="B71" s="4"/>
       <c r="C71" s="8"/>
       <c r="D71" s="8"/>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="3"/>
       <c r="B72" s="4"/>
       <c r="C72" s="8"/>
       <c r="D72" s="8"/>
     </row>
-    <row r="73" spans="1:4">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="3"/>
       <c r="B73" s="4"/>
       <c r="C73" s="8"/>
       <c r="D73" s="8"/>
     </row>
-    <row r="74" spans="1:4">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="3"/>
       <c r="B74" s="4"/>
       <c r="C74" s="8"/>
       <c r="D74" s="8"/>
     </row>
-    <row r="75" spans="1:4">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="3"/>
       <c r="B75" s="4"/>
       <c r="C75" s="8"/>
       <c r="D75" s="8"/>
     </row>
-    <row r="76" spans="1:4">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="3"/>
       <c r="B76" s="4"/>
       <c r="C76" s="8"/>
       <c r="D76" s="8"/>
     </row>
-    <row r="77" spans="1:4">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="3"/>
       <c r="B77" s="4"/>
       <c r="C77" s="8"/>
       <c r="D77" s="8"/>
     </row>
-    <row r="78" spans="1:4">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="3"/>
       <c r="B78" s="4"/>
       <c r="C78" s="8"/>
       <c r="D78" s="8"/>
     </row>
-    <row r="79" spans="1:4">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="3"/>
       <c r="B79" s="4"/>
       <c r="C79" s="8"/>
       <c r="D79" s="8"/>
     </row>
-    <row r="80" spans="1:4">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="3"/>
       <c r="B80" s="4"/>
       <c r="C80" s="8"/>
       <c r="D80" s="8"/>
     </row>
-    <row r="81" spans="1:4">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="3"/>
       <c r="B81" s="4"/>
       <c r="C81" s="8"/>
       <c r="D81" s="8"/>
     </row>
-    <row r="82" spans="1:4">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="3"/>
       <c r="B82" s="4"/>
       <c r="C82" s="8"/>
       <c r="D82" s="8"/>
     </row>
-    <row r="83" spans="1:4">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="3"/>
       <c r="B83" s="4"/>
       <c r="C83" s="8"/>
       <c r="D83" s="8"/>
     </row>
-    <row r="84" spans="1:4">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="3"/>
       <c r="B84" s="4"/>
       <c r="C84" s="8"/>
       <c r="D84" s="8"/>
     </row>
-    <row r="85" spans="1:4">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="3"/>
       <c r="B85" s="4"/>
       <c r="C85" s="8"/>
       <c r="D85" s="8"/>
     </row>
-    <row r="86" spans="1:4">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="3"/>
       <c r="B86" s="4"/>
       <c r="C86" s="8"/>
       <c r="D86" s="8"/>
     </row>
-    <row r="87" spans="1:4">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="3"/>
       <c r="B87" s="4"/>
       <c r="C87" s="8"/>
       <c r="D87" s="8"/>
     </row>
-    <row r="88" spans="1:4">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="3"/>
       <c r="B88" s="4"/>
       <c r="C88" s="8"/>
       <c r="D88" s="8"/>
     </row>
-    <row r="89" spans="1:4">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="3"/>
       <c r="B89" s="4"/>
       <c r="C89" s="8"/>
       <c r="D89" s="8"/>
     </row>
-    <row r="90" spans="1:4">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="3"/>
       <c r="B90" s="4"/>
       <c r="C90" s="8"/>
       <c r="D90" s="8"/>
     </row>
-    <row r="91" spans="1:4">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="3"/>
       <c r="B91" s="4"/>
       <c r="C91" s="8"/>
       <c r="D91" s="8"/>
     </row>
-    <row r="92" spans="1:4">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="3"/>
       <c r="B92" s="4"/>
       <c r="C92" s="8"/>
       <c r="D92" s="8"/>
     </row>
-    <row r="93" spans="1:4">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="3"/>
       <c r="B93" s="4"/>
       <c r="C93" s="8"/>
       <c r="D93" s="8"/>
     </row>
-    <row r="94" spans="1:4">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="3"/>
       <c r="B94" s="4"/>
       <c r="C94" s="8"/>
       <c r="D94" s="8"/>
     </row>
-    <row r="95" spans="1:4">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="3"/>
       <c r="B95" s="4"/>
       <c r="C95" s="8"/>
       <c r="D95" s="8"/>
     </row>
-    <row r="96" spans="1:4">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="3"/>
       <c r="B96" s="4"/>
       <c r="C96" s="8"/>
       <c r="D96" s="8"/>
     </row>
-    <row r="97" spans="1:4">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="3"/>
       <c r="B97" s="4"/>
       <c r="C97" s="8"/>
       <c r="D97" s="8"/>
     </row>
-    <row r="98" spans="1:4">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="3"/>
       <c r="B98" s="4"/>
       <c r="C98" s="8"/>
       <c r="D98" s="8"/>
     </row>
-    <row r="99" spans="1:4">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="3"/>
       <c r="B99" s="4"/>
       <c r="C99" s="8"/>
       <c r="D99" s="8"/>
     </row>
-    <row r="100" spans="1:4">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="3"/>
       <c r="B100" s="4"/>
       <c r="C100" s="8"/>
       <c r="D100" s="8"/>
     </row>
-    <row r="101" spans="1:4">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="3"/>
       <c r="B101" s="4"/>
       <c r="C101" s="8"/>
       <c r="D101" s="8"/>
     </row>
-    <row r="102" spans="1:4">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="3"/>
       <c r="B102" s="4"/>
       <c r="C102" s="8"/>
       <c r="D102" s="8"/>
     </row>
-    <row r="103" spans="1:4">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="3"/>
       <c r="B103" s="4"/>
       <c r="C103" s="8"/>
       <c r="D103" s="8"/>
     </row>
-    <row r="104" spans="1:4">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="3"/>
       <c r="B104" s="4"/>
       <c r="C104" s="8"/>
       <c r="D104" s="8"/>
     </row>
-    <row r="105" spans="1:4">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="3"/>
       <c r="B105" s="4"/>
       <c r="C105" s="8"/>
       <c r="D105" s="8"/>
     </row>
-    <row r="106" spans="1:4">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="3"/>
       <c r="B106" s="4"/>
       <c r="C106" s="8"/>
       <c r="D106" s="8"/>
     </row>
-    <row r="107" spans="1:4">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="3"/>
       <c r="B107" s="4"/>
       <c r="C107" s="8"/>
       <c r="D107" s="8"/>
     </row>
-    <row r="108" spans="1:4">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="3"/>
       <c r="B108" s="4"/>
       <c r="C108" s="8"/>
       <c r="D108" s="8"/>
     </row>
-    <row r="109" spans="1:4">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="3"/>
       <c r="B109" s="4"/>
       <c r="C109" s="8"/>
       <c r="D109" s="8"/>
     </row>
-    <row r="110" spans="1:4">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="3"/>
       <c r="B110" s="4"/>
       <c r="C110" s="8"/>
       <c r="D110" s="8"/>
     </row>
-    <row r="111" spans="1:4">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="3"/>
       <c r="B111" s="4"/>
       <c r="C111" s="8"/>
       <c r="D111" s="8"/>
     </row>
-    <row r="112" spans="1:4">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="3"/>
       <c r="B112" s="4"/>
       <c r="C112" s="8"/>
       <c r="D112" s="8"/>
     </row>
-    <row r="113" spans="1:4">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="3"/>
       <c r="B113" s="4"/>
       <c r="C113" s="8"/>
       <c r="D113" s="8"/>
     </row>
-    <row r="114" spans="1:4">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="3"/>
       <c r="B114" s="4"/>
       <c r="C114" s="8"/>
       <c r="D114" s="8"/>
     </row>
-    <row r="115" spans="1:4">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="3"/>
       <c r="B115" s="4"/>
       <c r="C115" s="8"/>
       <c r="D115" s="8"/>
     </row>
-    <row r="116" spans="1:4">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="3"/>
       <c r="B116" s="4"/>
       <c r="C116" s="8"/>
       <c r="D116" s="8"/>
     </row>
-    <row r="117" spans="1:4">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="3"/>
       <c r="B117" s="4"/>
       <c r="C117" s="8"/>
       <c r="D117" s="8"/>
     </row>
-    <row r="118" spans="1:4">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="3"/>
       <c r="B118" s="4"/>
       <c r="C118" s="8"/>
       <c r="D118" s="8"/>
     </row>
-    <row r="119" spans="1:4">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="3"/>
       <c r="B119" s="4"/>
       <c r="C119" s="8"/>
       <c r="D119" s="8"/>
     </row>
-    <row r="120" spans="1:4">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="3"/>
       <c r="B120" s="4"/>
       <c r="C120" s="8"/>
       <c r="D120" s="8"/>
     </row>
-    <row r="121" spans="1:4">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="3"/>
       <c r="B121" s="4"/>
       <c r="C121" s="8"/>
       <c r="D121" s="8"/>
     </row>
-    <row r="122" spans="1:4">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="3"/>
       <c r="B122" s="4"/>
       <c r="C122" s="8"/>
       <c r="D122" s="8"/>
     </row>
-    <row r="123" spans="1:4">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="3"/>
       <c r="B123" s="4"/>
       <c r="C123" s="8"/>
       <c r="D123" s="8"/>
     </row>
-    <row r="124" spans="1:4">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="3"/>
       <c r="B124" s="4"/>
       <c r="C124" s="8"/>
       <c r="D124" s="8"/>
     </row>
-    <row r="125" spans="1:4">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="3"/>
       <c r="B125" s="4"/>
       <c r="C125" s="8"/>
       <c r="D125" s="8"/>
     </row>
-    <row r="126" spans="1:4">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="3"/>
       <c r="B126" s="4"/>
       <c r="C126" s="8"/>
       <c r="D126" s="8"/>
     </row>
-    <row r="127" spans="1:4">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="3"/>
       <c r="B127" s="4"/>
       <c r="C127" s="8"/>
       <c r="D127" s="8"/>
     </row>
-    <row r="128" spans="1:4">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="3"/>
       <c r="B128" s="4"/>
       <c r="C128" s="8"/>
       <c r="D128" s="8"/>
     </row>
-    <row r="129" spans="1:4">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="3"/>
       <c r="B129" s="4"/>
       <c r="C129" s="8"/>
       <c r="D129" s="8"/>
     </row>
-    <row r="130" spans="1:4">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="3"/>
       <c r="B130" s="4"/>
       <c r="C130" s="8"/>
       <c r="D130" s="8"/>
     </row>
-    <row r="131" spans="1:4">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="3"/>
       <c r="B131" s="4"/>
       <c r="C131" s="8"/>
       <c r="D131" s="8"/>
     </row>
-    <row r="132" spans="1:4">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="3"/>
       <c r="B132" s="4"/>
       <c r="C132" s="8"/>
       <c r="D132" s="8"/>
     </row>
-    <row r="133" spans="1:4">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="3"/>
       <c r="B133" s="4"/>
       <c r="C133" s="8"/>
       <c r="D133" s="8"/>
     </row>
-    <row r="134" spans="1:4">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="3"/>
       <c r="B134" s="4"/>
       <c r="C134" s="8"/>
       <c r="D134" s="8"/>
     </row>
-    <row r="135" spans="1:4">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="3"/>
       <c r="B135" s="4"/>
       <c r="C135" s="8"/>
       <c r="D135" s="8"/>
     </row>
-    <row r="136" spans="1:4">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="3"/>
       <c r="B136" s="4"/>
       <c r="C136" s="8"/>
       <c r="D136" s="8"/>
     </row>
-    <row r="137" spans="1:4">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="3"/>
       <c r="B137" s="4"/>
       <c r="C137" s="8"/>
       <c r="D137" s="8"/>
     </row>
-    <row r="138" spans="1:4">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="3"/>
       <c r="B138" s="4"/>
       <c r="C138" s="8"/>
       <c r="D138" s="8"/>
     </row>
-    <row r="139" spans="1:4">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="3"/>
       <c r="B139" s="4"/>
       <c r="C139" s="8"/>
       <c r="D139" s="8"/>
     </row>
-    <row r="140" spans="1:4">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="3"/>
       <c r="B140" s="4"/>
       <c r="C140" s="8"/>
       <c r="D140" s="8"/>
     </row>
-    <row r="141" spans="1:4">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="3"/>
       <c r="B141" s="4"/>
       <c r="C141" s="8"/>
       <c r="D141" s="8"/>
     </row>
-    <row r="142" spans="1:4">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="9"/>
       <c r="B142" s="4"/>
       <c r="C142" s="8"/>
       <c r="D142" s="8"/>
     </row>
-    <row r="143" spans="1:4">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="9"/>
       <c r="B143" s="4"/>
       <c r="C143" s="8"/>
       <c r="D143" s="8"/>
     </row>
-    <row r="144" spans="1:4">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="9"/>
       <c r="B144" s="4"/>
       <c r="C144" s="8"/>
       <c r="D144" s="8"/>
     </row>
-    <row r="145" spans="1:4">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="9"/>
       <c r="B145" s="4"/>
       <c r="C145" s="8"/>
       <c r="D145" s="8"/>
     </row>
-    <row r="146" spans="1:4">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="9"/>
       <c r="B146" s="4"/>
       <c r="C146" s="8"/>
       <c r="D146" s="8"/>
     </row>
-    <row r="147" spans="1:4">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="9"/>
       <c r="B147" s="4"/>
       <c r="C147" s="8"/>
       <c r="D147" s="8"/>
     </row>
-    <row r="148" spans="1:4">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="9"/>
       <c r="B148" s="4"/>
       <c r="C148" s="8"/>
       <c r="D148" s="8"/>
     </row>
-    <row r="149" spans="1:4">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="9"/>
       <c r="B149" s="4"/>
       <c r="C149" s="8"/>
       <c r="D149" s="8"/>
     </row>
-    <row r="150" spans="1:4">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="9"/>
       <c r="B150" s="4"/>
       <c r="C150" s="8"/>
       <c r="D150" s="8"/>
     </row>
-    <row r="151" spans="1:4">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="9"/>
       <c r="B151" s="4"/>
       <c r="C151" s="8"/>
       <c r="D151" s="8"/>
     </row>
-    <row r="152" spans="1:4">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="3"/>
       <c r="B152" s="4"/>
       <c r="C152" s="8"/>
       <c r="D152" s="8"/>
     </row>
-    <row r="153" spans="1:4">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="3"/>
       <c r="B153" s="4"/>
       <c r="C153" s="8"/>
       <c r="D153" s="8"/>
     </row>
-    <row r="154" spans="1:4">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="3"/>
       <c r="B154" s="4"/>
       <c r="C154" s="8"/>
       <c r="D154" s="8"/>
     </row>
-    <row r="155" spans="1:4">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="3"/>
       <c r="B155" s="4"/>
       <c r="C155" s="8"/>
       <c r="D155" s="8"/>
     </row>
-    <row r="156" spans="1:4">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" s="3"/>
       <c r="B156" s="4"/>
       <c r="C156" s="8"/>
       <c r="D156" s="8"/>
     </row>
-    <row r="157" spans="1:4">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="4"/>
       <c r="B157" s="5"/>
     </row>
-    <row r="158" spans="1:4">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" s="4"/>
       <c r="B158" s="5"/>
     </row>
-    <row r="159" spans="1:4">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="4"/>
       <c r="B159" s="5"/>
     </row>
-    <row r="160" spans="1:4">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="4"/>
       <c r="B160" s="5"/>
     </row>
-    <row r="161" spans="1:2">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" s="4"/>
       <c r="B161" s="5"/>
     </row>
-    <row r="162" spans="1:2">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" s="4"/>
       <c r="B162" s="5"/>
     </row>
-    <row r="163" spans="1:2">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" s="4"/>
       <c r="B163" s="5"/>
     </row>
-    <row r="164" spans="1:2">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" s="4"/>
       <c r="B164" s="5"/>
     </row>
-    <row r="165" spans="1:2">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" s="4"/>
       <c r="B165" s="5"/>
     </row>
-    <row r="166" spans="1:2">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" s="4"/>
       <c r="B166" s="5"/>
     </row>
-    <row r="167" spans="1:2">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" s="4"/>
       <c r="B167" s="5"/>
     </row>
-    <row r="168" spans="1:2">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" s="4"/>
       <c r="B168" s="5"/>
     </row>
-    <row r="169" spans="1:2">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" s="4"/>
       <c r="B169" s="5"/>
     </row>
-    <row r="170" spans="1:2">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" s="4"/>
       <c r="B170" s="5"/>
     </row>
-    <row r="171" spans="1:2">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" s="4"/>
       <c r="B171" s="5"/>
     </row>
-    <row r="172" spans="1:2">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" s="4"/>
       <c r="B172" s="5"/>
     </row>
-    <row r="173" spans="1:2">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" s="4"/>
       <c r="B173" s="5"/>
     </row>
-    <row r="174" spans="1:2">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" s="4"/>
       <c r="B174" s="5"/>
     </row>
-    <row r="175" spans="1:2">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" s="4"/>
       <c r="B175" s="5"/>
     </row>
-    <row r="176" spans="1:2">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" s="4"/>
       <c r="B176" s="5"/>
     </row>
-    <row r="177" spans="1:2">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" s="4"/>
       <c r="B177" s="5"/>
     </row>
-    <row r="178" spans="1:2">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" s="4"/>
       <c r="B178" s="5"/>
     </row>
-    <row r="179" spans="1:2">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" s="4"/>
       <c r="B179" s="5"/>
     </row>
-    <row r="180" spans="1:2">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" s="4"/>
       <c r="B180" s="5"/>
     </row>
-    <row r="181" spans="1:2">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" s="4"/>
       <c r="B181" s="5"/>
     </row>
-    <row r="182" spans="1:2">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" s="4"/>
       <c r="B182" s="5"/>
     </row>
-    <row r="183" spans="1:2">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" s="4"/>
       <c r="B183" s="5"/>
     </row>
-    <row r="184" spans="1:2">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" s="4"/>
       <c r="B184" s="5"/>
     </row>
-    <row r="185" spans="1:2">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" s="4"/>
       <c r="B185" s="5"/>
     </row>
-    <row r="186" spans="1:2">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" s="4"/>
       <c r="B186" s="5"/>
     </row>
-    <row r="187" spans="1:2">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" s="4"/>
       <c r="B187" s="5"/>
     </row>
-    <row r="188" spans="1:2">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" s="4"/>
       <c r="B188" s="5"/>
     </row>
-    <row r="189" spans="1:2">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" s="4"/>
       <c r="B189" s="5"/>
     </row>
-    <row r="190" spans="1:2">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" s="4"/>
       <c r="B190" s="5"/>
     </row>
-    <row r="191" spans="1:2">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" s="4"/>
       <c r="B191" s="5"/>
     </row>
-    <row r="192" spans="1:2">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" s="4"/>
       <c r="B192" s="5"/>
     </row>
-    <row r="193" spans="1:2">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" s="4"/>
       <c r="B193" s="5"/>
     </row>
-    <row r="194" spans="1:2">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" s="4"/>
       <c r="B194" s="5"/>
     </row>
-    <row r="195" spans="1:2">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" s="4"/>
       <c r="B195" s="5"/>
     </row>
-    <row r="196" spans="1:2">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" s="4"/>
       <c r="B196" s="5"/>
     </row>
-    <row r="197" spans="1:2">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" s="4"/>
       <c r="B197" s="5"/>
     </row>
-    <row r="198" spans="1:2">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" s="4"/>
       <c r="B198" s="5"/>
     </row>
-    <row r="199" spans="1:2">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" s="4"/>
       <c r="B199" s="5"/>
     </row>
-    <row r="200" spans="1:2">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" s="4"/>
       <c r="B200" s="5"/>
     </row>
-    <row r="201" spans="1:2">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" s="4"/>
       <c r="B201" s="5"/>
     </row>
-    <row r="202" spans="1:2">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" s="4"/>
       <c r="B202" s="5"/>
     </row>
-    <row r="203" spans="1:2">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" s="4"/>
       <c r="B203" s="5"/>
     </row>
-    <row r="204" spans="1:2">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" s="4"/>
       <c r="B204" s="5"/>
     </row>
-    <row r="205" spans="1:2">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" s="4"/>
       <c r="B205" s="5"/>
     </row>
-    <row r="206" spans="1:2">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" s="4"/>
       <c r="B206" s="5"/>
     </row>
-    <row r="207" spans="1:2">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" s="4"/>
       <c r="B207" s="5"/>
     </row>
-    <row r="208" spans="1:2">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" s="4"/>
       <c r="B208" s="5"/>
     </row>
-    <row r="209" spans="1:2">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" s="4"/>
       <c r="B209" s="5"/>
     </row>
-    <row r="210" spans="1:2">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" s="4"/>
       <c r="B210" s="5"/>
     </row>
-    <row r="211" spans="1:2">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" s="4"/>
       <c r="B211" s="5"/>
     </row>
-    <row r="212" spans="1:2">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" s="4"/>
       <c r="B212" s="5"/>
     </row>
-    <row r="213" spans="1:2">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" s="4"/>
       <c r="B213" s="5"/>
     </row>
-    <row r="214" spans="1:2">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" s="4"/>
       <c r="B214" s="5"/>
     </row>
-    <row r="215" spans="1:2">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" s="4"/>
       <c r="B215" s="5"/>
     </row>
-    <row r="216" spans="1:2">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" s="4"/>
       <c r="B216" s="5"/>
     </row>
-    <row r="217" spans="1:2">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" s="4"/>
       <c r="B217" s="5"/>
     </row>
-    <row r="218" spans="1:2">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" s="4"/>
       <c r="B218" s="5"/>
     </row>
-    <row r="219" spans="1:2">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" s="4"/>
       <c r="B219" s="5"/>
     </row>
-    <row r="220" spans="1:2">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" s="4"/>
       <c r="B220" s="5"/>
     </row>
-    <row r="221" spans="1:2">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" s="4"/>
       <c r="B221" s="5"/>
     </row>
-    <row r="222" spans="1:2">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" s="4"/>
       <c r="B222" s="5"/>
     </row>
-    <row r="223" spans="1:2">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" s="4"/>
       <c r="B223" s="5"/>
     </row>
-    <row r="224" spans="1:2">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" s="4"/>
       <c r="B224" s="5"/>
     </row>
-    <row r="225" spans="1:2">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" s="4"/>
       <c r="B225" s="5"/>
     </row>
-    <row r="226" spans="1:2">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" s="4"/>
       <c r="B226" s="5"/>
     </row>
-    <row r="227" spans="1:2">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" s="4"/>
       <c r="B227" s="5"/>
     </row>
-    <row r="228" spans="1:2">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" s="4"/>
       <c r="B228" s="5"/>
     </row>
-    <row r="229" spans="1:2">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" s="4"/>
       <c r="B229" s="5"/>
     </row>
-    <row r="230" spans="1:2">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" s="4"/>
       <c r="B230" s="5"/>
     </row>
-    <row r="231" spans="1:2">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" s="4"/>
       <c r="B231" s="5"/>
     </row>
-    <row r="232" spans="1:2">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" s="4"/>
       <c r="B232" s="5"/>
     </row>
-    <row r="233" spans="1:2">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" s="4"/>
       <c r="B233" s="5"/>
     </row>
-    <row r="234" spans="1:2">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" s="4"/>
       <c r="B234" s="5"/>
     </row>
-    <row r="235" spans="1:2">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" s="4"/>
       <c r="B235" s="5"/>
     </row>
-    <row r="236" spans="1:2">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" s="4"/>
       <c r="B236" s="5"/>
     </row>
-    <row r="237" spans="1:2">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" s="4"/>
       <c r="B237" s="5"/>
     </row>
-    <row r="238" spans="1:2">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" s="4"/>
       <c r="B238" s="5"/>
     </row>
-    <row r="239" spans="1:2">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" s="4"/>
       <c r="B239" s="5"/>
     </row>
-    <row r="240" spans="1:2">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" s="3"/>
       <c r="B240" s="5"/>
     </row>
-    <row r="241" spans="1:2">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" s="3"/>
       <c r="B241" s="5"/>
     </row>
-    <row r="242" spans="1:2">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" s="3"/>
       <c r="B242" s="5"/>
     </row>
-    <row r="243" spans="1:2">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" s="3"/>
       <c r="B243" s="5"/>
     </row>
-    <row r="244" spans="1:2">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" s="3"/>
       <c r="B244" s="5"/>
     </row>
-    <row r="245" spans="1:2">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" s="3"/>
       <c r="B245" s="5"/>
     </row>
-    <row r="246" spans="1:2">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" s="3"/>
       <c r="B246" s="5"/>
     </row>
-    <row r="247" spans="1:2">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" s="3"/>
       <c r="B247" s="5"/>
     </row>
-    <row r="248" spans="1:2">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248" s="3"/>
       <c r="B248" s="5"/>
     </row>
-    <row r="249" spans="1:2">
+    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" s="3"/>
       <c r="B249" s="5"/>
     </row>
-    <row r="250" spans="1:2">
+    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250" s="3"/>
       <c r="B250" s="5"/>
     </row>
-    <row r="251" spans="1:2">
+    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251" s="3"/>
       <c r="B251" s="5"/>
     </row>
-    <row r="252" spans="1:2">
+    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A252" s="3"/>
       <c r="B252" s="5"/>
     </row>
-    <row r="253" spans="1:2">
+    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253" s="3"/>
       <c r="B253" s="5"/>
     </row>
@@ -4203,13 +4212,39 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D9CBEFE-8C4C-4054-8E02-CA457E93B4C8}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D9CBEFE-8C4C-4054-8E02-CA457E93B4C8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
+    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F0D7176-14CB-4F63-BBB4-5E9CDAB9112D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F0D7176-14CB-4F63-BBB4-5E9CDAB9112D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
+    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C05FF1B-7508-40EF-8319-E993EA07F007}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C05FF1B-7508-40EF-8319-E993EA07F007}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
same changes as in KORA S1
</commit_message>
<xml_diff>
--- a/rmonize/data_dictionary/DD_KORA_S3_P1.xlsx
+++ b/rmonize/data_dictionary/DD_KORA_S3_P1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\rmonize\data_dictionary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\NFDI4Health\TA5\Pilotprojekte\Harmonisierung\HarmonizR\use-cases-harmonisation\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB833AE-C591-4F2D-A9C7-4D51C3AC7029}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E9DE011D-A311-4D6F-B189-DDE6FF519F11}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12228" xr2:uid="{1200B70D-B446-4CDA-99A8-3FD394D791D2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{1200B70D-B446-4CDA-99A8-3FD394D791D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="224">
   <si>
     <t>index</t>
   </si>
@@ -85,6 +96,12 @@
     <t>decimal</t>
   </si>
   <si>
+    <t>dkcal</t>
+  </si>
+  <si>
+    <t>energy</t>
+  </si>
+  <si>
     <t>DV410</t>
   </si>
   <si>
@@ -646,6 +663,12 @@
     <t>fruit wine</t>
   </si>
   <si>
+    <t>DV491</t>
+  </si>
+  <si>
+    <t>dry legumes</t>
+  </si>
+  <si>
     <t>variable</t>
   </si>
   <si>
@@ -686,12 +709,6 @@
   </si>
   <si>
     <t>unknown</t>
-  </si>
-  <si>
-    <t>dry legumes</t>
-  </si>
-  <si>
-    <t>DV491</t>
   </si>
 </sst>
 </file>
@@ -1098,21 +1115,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08A73012-5CAD-43B9-A281-79101DF4E1E0}">
-  <dimension ref="A1:F101"/>
+  <dimension ref="A1:F102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31:D40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B113" sqref="B113"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" style="9"/>
-    <col min="2" max="2" width="26.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.88671875" style="9" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" style="9"/>
+    <col min="1" max="1" width="11.42578125" style="9"/>
+    <col min="2" max="2" width="26.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.85546875" style="9" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1126,7 +1143,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
         <v>1</v>
       </c>
@@ -1140,7 +1157,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <v>2</v>
       </c>
@@ -1154,7 +1171,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>3</v>
       </c>
@@ -1168,7 +1185,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>4</v>
       </c>
@@ -1182,7 +1199,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>5</v>
       </c>
@@ -1196,7 +1213,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>6</v>
       </c>
@@ -1210,7 +1227,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>7</v>
       </c>
@@ -1221,10 +1238,10 @@
         <v>20</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>8</v>
       </c>
@@ -1235,10 +1252,10 @@
         <v>22</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>9</v>
       </c>
@@ -1249,10 +1266,10 @@
         <v>24</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>10</v>
       </c>
@@ -1263,10 +1280,10 @@
         <v>26</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>11</v>
       </c>
@@ -1277,10 +1294,10 @@
         <v>28</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>12</v>
       </c>
@@ -1291,10 +1308,10 @@
         <v>30</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>13</v>
       </c>
@@ -1305,10 +1322,10 @@
         <v>32</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>14</v>
       </c>
@@ -1319,94 +1336,94 @@
         <v>34</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>15</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D16" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D17" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D18" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="D19" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D19" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
         <v>19</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="3" t="s">
         <v>43</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D20" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
         <v>20</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="9" t="s">
         <v>45</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="D21" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D21" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
         <v>21</v>
       </c>
@@ -1416,11 +1433,11 @@
       <c r="C22" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="D22" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D22" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
         <v>22</v>
       </c>
@@ -1430,11 +1447,11 @@
       <c r="C23" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="D23" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D23" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
         <v>23</v>
       </c>
@@ -1444,11 +1461,11 @@
       <c r="C24" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="D24" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D24" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
         <v>24</v>
       </c>
@@ -1458,11 +1475,11 @@
       <c r="C25" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="D25" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D25" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="9">
         <v>25</v>
       </c>
@@ -1472,81 +1489,81 @@
       <c r="C26" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="D26" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D26" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="9">
         <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="D27" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D27" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="9">
         <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C28" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D28" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D28" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="9">
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="D29" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D29" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="9">
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="C30" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D30" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D30" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="9">
         <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D31" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D31" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="9">
         <v>31</v>
       </c>
@@ -1556,11 +1573,11 @@
       <c r="C32" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D32" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D32" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="9">
         <v>32</v>
       </c>
@@ -1570,11 +1587,11 @@
       <c r="C33" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D33" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D33" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="9">
         <v>33</v>
       </c>
@@ -1584,11 +1601,11 @@
       <c r="C34" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D34" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D34" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="9">
         <v>34</v>
       </c>
@@ -1598,25 +1615,25 @@
       <c r="C35" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D35" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D35" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="9">
         <v>35</v>
       </c>
-      <c r="B36" s="9" t="s">
+      <c r="B36" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C36" s="9" t="s">
+      <c r="C36" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D36" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D36" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="9">
         <v>36</v>
       </c>
@@ -1626,25 +1643,25 @@
       <c r="C37" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D37" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D37" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="9">
         <v>37</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="9" t="s">
         <v>79</v>
       </c>
       <c r="C38" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="D38" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D38" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="9">
         <v>38</v>
       </c>
@@ -1654,11 +1671,11 @@
       <c r="C39" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="D39" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D39" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="9">
         <v>39</v>
       </c>
@@ -1668,11 +1685,11 @@
       <c r="C40" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="D40" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D40" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="9">
         <v>40</v>
       </c>
@@ -1682,25 +1699,25 @@
       <c r="C41" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="D41" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D41" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="9">
         <v>41</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C42" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="D42" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D42" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="9">
         <v>42</v>
       </c>
@@ -1710,11 +1727,11 @@
       <c r="C43" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D43" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D43" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="9">
         <v>43</v>
       </c>
@@ -1724,11 +1741,11 @@
       <c r="C44" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D44" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D44" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="9">
         <v>44</v>
       </c>
@@ -1738,11 +1755,11 @@
       <c r="C45" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D45" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D45" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="9">
         <v>45</v>
       </c>
@@ -1752,11 +1769,11 @@
       <c r="C46" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="D46" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D46" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="9">
         <v>46</v>
       </c>
@@ -1766,25 +1783,25 @@
       <c r="C47" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="D47" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D47" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="9">
         <v>47</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C48" s="9" t="s">
+      <c r="C48" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="D48" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D48" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="9">
         <v>48</v>
       </c>
@@ -1794,11 +1811,11 @@
       <c r="C49" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="D49" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D49" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="9">
         <v>49</v>
       </c>
@@ -1808,11 +1825,11 @@
       <c r="C50" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="D50" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D50" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="9">
         <v>50</v>
       </c>
@@ -1822,11 +1839,11 @@
       <c r="C51" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="D51" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D51" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="9">
         <v>51</v>
       </c>
@@ -1836,39 +1853,39 @@
       <c r="C52" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="D52" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D52" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="9">
         <v>52</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="C53" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="D53" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D53" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="9">
         <v>53</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C54" s="9" t="s">
+      <c r="C54" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="D54" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D54" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="9">
         <v>54</v>
       </c>
@@ -1878,11 +1895,11 @@
       <c r="C55" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="D55" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D55" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="9">
         <v>55</v>
       </c>
@@ -1892,11 +1909,11 @@
       <c r="C56" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="D56" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D56" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="9">
         <v>56</v>
       </c>
@@ -1906,39 +1923,39 @@
       <c r="C57" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D57" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D57" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="9">
         <v>57</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="C58" s="3" t="s">
+      <c r="C58" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="D58" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D58" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="9">
         <v>58</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C59" s="9" t="s">
+      <c r="C59" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="D59" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D59" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="9">
         <v>59</v>
       </c>
@@ -1948,11 +1965,11 @@
       <c r="C60" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="D60" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D60" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="9">
         <v>60</v>
       </c>
@@ -1962,67 +1979,67 @@
       <c r="C61" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="D61" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D61" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="9">
         <v>61</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="C62" s="6" t="s">
+      <c r="C62" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="D62" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D62" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="9">
         <v>62</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C63" s="3" t="s">
+      <c r="C63" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="D63" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D63" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="9">
         <v>63</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="C64" s="6" t="s">
+      <c r="C64" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="D64" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D64" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="9">
         <v>64</v>
       </c>
-      <c r="B65" s="9" t="s">
+      <c r="B65" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="C65" s="9" t="s">
+      <c r="C65" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="D65" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D65" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="9">
         <v>65</v>
       </c>
@@ -2032,11 +2049,11 @@
       <c r="C66" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="D66" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D66" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="9">
         <v>66</v>
       </c>
@@ -2046,11 +2063,11 @@
       <c r="C67" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="D67" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D67" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="9">
         <v>67</v>
       </c>
@@ -2060,11 +2077,11 @@
       <c r="C68" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="D68" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D68" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="9">
         <v>68</v>
       </c>
@@ -2074,11 +2091,11 @@
       <c r="C69" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="D69" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D69" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="9">
         <v>69</v>
       </c>
@@ -2088,11 +2105,11 @@
       <c r="C70" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="D70" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D70" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="9">
         <v>70</v>
       </c>
@@ -2102,11 +2119,11 @@
       <c r="C71" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="D71" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D71" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="9">
         <v>71</v>
       </c>
@@ -2116,11 +2133,11 @@
       <c r="C72" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="D72" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D72" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="9">
         <v>72</v>
       </c>
@@ -2130,11 +2147,11 @@
       <c r="C73" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="D73" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D73" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="9">
         <v>73</v>
       </c>
@@ -2144,11 +2161,11 @@
       <c r="C74" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="D74" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D74" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="9">
         <v>74</v>
       </c>
@@ -2158,11 +2175,11 @@
       <c r="C75" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="D75" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D75" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="9">
         <v>75</v>
       </c>
@@ -2172,11 +2189,11 @@
       <c r="C76" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="D76" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D76" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="9">
         <v>76</v>
       </c>
@@ -2186,11 +2203,11 @@
       <c r="C77" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="D77" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D77" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="9">
         <v>77</v>
       </c>
@@ -2200,11 +2217,11 @@
       <c r="C78" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="D78" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D78" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="9">
         <v>78</v>
       </c>
@@ -2214,11 +2231,11 @@
       <c r="C79" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="D79" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D79" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="9">
         <v>79</v>
       </c>
@@ -2228,11 +2245,11 @@
       <c r="C80" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="D80" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D80" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="9">
         <v>80</v>
       </c>
@@ -2242,11 +2259,11 @@
       <c r="C81" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="D81" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D81" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="9">
         <v>81</v>
       </c>
@@ -2256,25 +2273,25 @@
       <c r="C82" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="D82" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D82" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="9">
         <v>82</v>
       </c>
-      <c r="B83" s="3" t="s">
+      <c r="B83" s="9" t="s">
         <v>169</v>
       </c>
       <c r="C83" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="D83" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D83" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="9">
         <v>83</v>
       </c>
@@ -2284,11 +2301,11 @@
       <c r="C84" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="D84" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D84" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="9">
         <v>84</v>
       </c>
@@ -2298,67 +2315,67 @@
       <c r="C85" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="D85" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D85" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="9">
         <v>85</v>
       </c>
-      <c r="B86" s="9" t="s">
+      <c r="B86" s="3" t="s">
         <v>175</v>
       </c>
       <c r="C86" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="D86" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D86" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="9">
         <v>86</v>
       </c>
       <c r="B87" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="C87" s="2" t="s">
+      <c r="C87" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="D87" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D87" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="9">
         <v>87</v>
       </c>
-      <c r="B88" s="3" t="s">
+      <c r="B88" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="C88" s="9" t="s">
+      <c r="C88" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="D88" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D88" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="9">
         <v>88</v>
       </c>
-      <c r="B89" s="9" t="s">
+      <c r="B89" s="3" t="s">
         <v>181</v>
       </c>
       <c r="C89" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="D89" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D89" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="9">
         <v>89</v>
       </c>
@@ -2368,11 +2385,11 @@
       <c r="C90" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="D90" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D90" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="9">
         <v>90</v>
       </c>
@@ -2382,28 +2399,28 @@
       <c r="C91" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="D91" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F91" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D91" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="9">
         <v>91</v>
       </c>
       <c r="B92" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="C92" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="C92" s="9" t="s">
+      <c r="D92" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F92" t="s">
         <v>189</v>
       </c>
-      <c r="D92" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="9">
         <v>92</v>
       </c>
@@ -2413,11 +2430,11 @@
       <c r="C93" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="D93" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D93" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="9">
         <v>93</v>
       </c>
@@ -2427,11 +2444,11 @@
       <c r="C94" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="D94" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D94" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="9">
         <v>94</v>
       </c>
@@ -2441,11 +2458,11 @@
       <c r="C95" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="D95" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D95" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="9">
         <v>95</v>
       </c>
@@ -2455,11 +2472,11 @@
       <c r="C96" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="D96" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D96" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="9">
         <v>96</v>
       </c>
@@ -2469,11 +2486,11 @@
       <c r="C97" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="D97" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D97" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="9">
         <v>97</v>
       </c>
@@ -2483,11 +2500,11 @@
       <c r="C98" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="D98" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D98" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="9">
         <v>98</v>
       </c>
@@ -2497,11 +2514,11 @@
       <c r="C99" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="D99" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D99" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="9">
         <v>99</v>
       </c>
@@ -2511,22 +2528,36 @@
       <c r="C100" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="D100" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D100" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="9">
         <v>100</v>
       </c>
       <c r="B101" s="9" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="C101" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="D101" s="9" t="s">
-        <v>9</v>
+        <v>207</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="9">
+        <v>101</v>
+      </c>
+      <c r="B102" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="C102" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -2543,16 +2574,16 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -2561,11 +2592,11 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>7</v>
       </c>
@@ -2573,10 +2604,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>7</v>
       </c>
@@ -2584,10 +2615,10 @@
         <v>2</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>12</v>
       </c>
@@ -2595,10 +2626,10 @@
         <v>0</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>12</v>
       </c>
@@ -2606,10 +2637,10 @@
         <v>1</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>12</v>
       </c>
@@ -2617,10 +2648,10 @@
         <v>2</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>12</v>
       </c>
@@ -2628,10 +2659,10 @@
         <v>3</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>12</v>
       </c>
@@ -2639,10 +2670,10 @@
         <v>4</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>12</v>
       </c>
@@ -2650,10 +2681,10 @@
         <v>5</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>14</v>
       </c>
@@ -2661,10 +2692,10 @@
         <v>1</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>14</v>
       </c>
@@ -2672,10 +2703,10 @@
         <v>2</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>14</v>
       </c>
@@ -2683,10 +2714,10 @@
         <v>3</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>14</v>
       </c>
@@ -2694,1252 +2725,1252 @@
         <v>4</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="4"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="4"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="4"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="4"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="4"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="4"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="4"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="4"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="4"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="4"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="4"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="4"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="4"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="4"/>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="4"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="4"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="4"/>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="4"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="4"/>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="4"/>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="4"/>
       <c r="C34" s="8"/>
       <c r="D34" s="8"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="4"/>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="4"/>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="4"/>
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="4"/>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="4"/>
       <c r="C39" s="8"/>
       <c r="D39" s="8"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="4"/>
       <c r="C40" s="8"/>
       <c r="D40" s="8"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="4"/>
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="4"/>
       <c r="C42" s="8"/>
       <c r="D42" s="8"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
       <c r="B43" s="4"/>
       <c r="C43" s="8"/>
       <c r="D43" s="8"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
       <c r="B44" s="4"/>
       <c r="C44" s="8"/>
       <c r="D44" s="8"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
       <c r="B45" s="4"/>
       <c r="C45" s="8"/>
       <c r="D45" s="8"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
       <c r="B46" s="4"/>
       <c r="C46" s="8"/>
       <c r="D46" s="8"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
       <c r="B47" s="4"/>
       <c r="C47" s="8"/>
       <c r="D47" s="8"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" s="4"/>
       <c r="C48" s="8"/>
       <c r="D48" s="8"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
       <c r="B49" s="4"/>
       <c r="C49" s="8"/>
       <c r="D49" s="8"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
       <c r="B50" s="4"/>
       <c r="C50" s="8"/>
       <c r="D50" s="8"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
       <c r="B51" s="4"/>
       <c r="C51" s="8"/>
       <c r="D51" s="8"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
       <c r="B52" s="4"/>
       <c r="C52" s="8"/>
       <c r="D52" s="8"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="3"/>
       <c r="B53" s="4"/>
       <c r="C53" s="8"/>
       <c r="D53" s="8"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
       <c r="B54" s="4"/>
       <c r="C54" s="8"/>
       <c r="D54" s="8"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="3"/>
       <c r="B55" s="4"/>
       <c r="C55" s="8"/>
       <c r="D55" s="8"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
       <c r="B56" s="4"/>
       <c r="C56" s="8"/>
       <c r="D56" s="8"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="3"/>
       <c r="B57" s="4"/>
       <c r="C57" s="8"/>
       <c r="D57" s="8"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="3"/>
       <c r="B58" s="4"/>
       <c r="C58" s="8"/>
       <c r="D58" s="8"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="3"/>
       <c r="B59" s="4"/>
       <c r="C59" s="8"/>
       <c r="D59" s="8"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="3"/>
       <c r="B60" s="4"/>
       <c r="C60" s="8"/>
       <c r="D60" s="8"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="3"/>
       <c r="B61" s="4"/>
       <c r="C61" s="8"/>
       <c r="D61" s="8"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
       <c r="B62" s="4"/>
       <c r="C62" s="8"/>
       <c r="D62" s="8"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="3"/>
       <c r="B63" s="4"/>
       <c r="C63" s="8"/>
       <c r="D63" s="8"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="3"/>
       <c r="B64" s="4"/>
       <c r="C64" s="8"/>
       <c r="D64" s="8"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="3"/>
       <c r="B65" s="4"/>
       <c r="C65" s="8"/>
       <c r="D65" s="8"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="3"/>
       <c r="B66" s="4"/>
       <c r="C66" s="8"/>
       <c r="D66" s="8"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="3"/>
       <c r="B67" s="4"/>
       <c r="C67" s="8"/>
       <c r="D67" s="8"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
       <c r="B68" s="4"/>
       <c r="C68" s="8"/>
       <c r="D68" s="8"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="3"/>
       <c r="B69" s="4"/>
       <c r="C69" s="8"/>
       <c r="D69" s="8"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="3"/>
       <c r="B70" s="4"/>
       <c r="C70" s="8"/>
       <c r="D70" s="8"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="3"/>
       <c r="B71" s="4"/>
       <c r="C71" s="8"/>
       <c r="D71" s="8"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="3"/>
       <c r="B72" s="4"/>
       <c r="C72" s="8"/>
       <c r="D72" s="8"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="3"/>
       <c r="B73" s="4"/>
       <c r="C73" s="8"/>
       <c r="D73" s="8"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="3"/>
       <c r="B74" s="4"/>
       <c r="C74" s="8"/>
       <c r="D74" s="8"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="3"/>
       <c r="B75" s="4"/>
       <c r="C75" s="8"/>
       <c r="D75" s="8"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="3"/>
       <c r="B76" s="4"/>
       <c r="C76" s="8"/>
       <c r="D76" s="8"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="3"/>
       <c r="B77" s="4"/>
       <c r="C77" s="8"/>
       <c r="D77" s="8"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="3"/>
       <c r="B78" s="4"/>
       <c r="C78" s="8"/>
       <c r="D78" s="8"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="3"/>
       <c r="B79" s="4"/>
       <c r="C79" s="8"/>
       <c r="D79" s="8"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="3"/>
       <c r="B80" s="4"/>
       <c r="C80" s="8"/>
       <c r="D80" s="8"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="3"/>
       <c r="B81" s="4"/>
       <c r="C81" s="8"/>
       <c r="D81" s="8"/>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="3"/>
       <c r="B82" s="4"/>
       <c r="C82" s="8"/>
       <c r="D82" s="8"/>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="3"/>
       <c r="B83" s="4"/>
       <c r="C83" s="8"/>
       <c r="D83" s="8"/>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="3"/>
       <c r="B84" s="4"/>
       <c r="C84" s="8"/>
       <c r="D84" s="8"/>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="3"/>
       <c r="B85" s="4"/>
       <c r="C85" s="8"/>
       <c r="D85" s="8"/>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="3"/>
       <c r="B86" s="4"/>
       <c r="C86" s="8"/>
       <c r="D86" s="8"/>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="3"/>
       <c r="B87" s="4"/>
       <c r="C87" s="8"/>
       <c r="D87" s="8"/>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="3"/>
       <c r="B88" s="4"/>
       <c r="C88" s="8"/>
       <c r="D88" s="8"/>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="3"/>
       <c r="B89" s="4"/>
       <c r="C89" s="8"/>
       <c r="D89" s="8"/>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="3"/>
       <c r="B90" s="4"/>
       <c r="C90" s="8"/>
       <c r="D90" s="8"/>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="3"/>
       <c r="B91" s="4"/>
       <c r="C91" s="8"/>
       <c r="D91" s="8"/>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="3"/>
       <c r="B92" s="4"/>
       <c r="C92" s="8"/>
       <c r="D92" s="8"/>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="3"/>
       <c r="B93" s="4"/>
       <c r="C93" s="8"/>
       <c r="D93" s="8"/>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="3"/>
       <c r="B94" s="4"/>
       <c r="C94" s="8"/>
       <c r="D94" s="8"/>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="3"/>
       <c r="B95" s="4"/>
       <c r="C95" s="8"/>
       <c r="D95" s="8"/>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="3"/>
       <c r="B96" s="4"/>
       <c r="C96" s="8"/>
       <c r="D96" s="8"/>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="3"/>
       <c r="B97" s="4"/>
       <c r="C97" s="8"/>
       <c r="D97" s="8"/>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="3"/>
       <c r="B98" s="4"/>
       <c r="C98" s="8"/>
       <c r="D98" s="8"/>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="3"/>
       <c r="B99" s="4"/>
       <c r="C99" s="8"/>
       <c r="D99" s="8"/>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="3"/>
       <c r="B100" s="4"/>
       <c r="C100" s="8"/>
       <c r="D100" s="8"/>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="3"/>
       <c r="B101" s="4"/>
       <c r="C101" s="8"/>
       <c r="D101" s="8"/>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="3"/>
       <c r="B102" s="4"/>
       <c r="C102" s="8"/>
       <c r="D102" s="8"/>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="3"/>
       <c r="B103" s="4"/>
       <c r="C103" s="8"/>
       <c r="D103" s="8"/>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="3"/>
       <c r="B104" s="4"/>
       <c r="C104" s="8"/>
       <c r="D104" s="8"/>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="3"/>
       <c r="B105" s="4"/>
       <c r="C105" s="8"/>
       <c r="D105" s="8"/>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="3"/>
       <c r="B106" s="4"/>
       <c r="C106" s="8"/>
       <c r="D106" s="8"/>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="3"/>
       <c r="B107" s="4"/>
       <c r="C107" s="8"/>
       <c r="D107" s="8"/>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="3"/>
       <c r="B108" s="4"/>
       <c r="C108" s="8"/>
       <c r="D108" s="8"/>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="3"/>
       <c r="B109" s="4"/>
       <c r="C109" s="8"/>
       <c r="D109" s="8"/>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="3"/>
       <c r="B110" s="4"/>
       <c r="C110" s="8"/>
       <c r="D110" s="8"/>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="3"/>
       <c r="B111" s="4"/>
       <c r="C111" s="8"/>
       <c r="D111" s="8"/>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="3"/>
       <c r="B112" s="4"/>
       <c r="C112" s="8"/>
       <c r="D112" s="8"/>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="3"/>
       <c r="B113" s="4"/>
       <c r="C113" s="8"/>
       <c r="D113" s="8"/>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="3"/>
       <c r="B114" s="4"/>
       <c r="C114" s="8"/>
       <c r="D114" s="8"/>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="3"/>
       <c r="B115" s="4"/>
       <c r="C115" s="8"/>
       <c r="D115" s="8"/>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="3"/>
       <c r="B116" s="4"/>
       <c r="C116" s="8"/>
       <c r="D116" s="8"/>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="3"/>
       <c r="B117" s="4"/>
       <c r="C117" s="8"/>
       <c r="D117" s="8"/>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="3"/>
       <c r="B118" s="4"/>
       <c r="C118" s="8"/>
       <c r="D118" s="8"/>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="3"/>
       <c r="B119" s="4"/>
       <c r="C119" s="8"/>
       <c r="D119" s="8"/>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="3"/>
       <c r="B120" s="4"/>
       <c r="C120" s="8"/>
       <c r="D120" s="8"/>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="3"/>
       <c r="B121" s="4"/>
       <c r="C121" s="8"/>
       <c r="D121" s="8"/>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="3"/>
       <c r="B122" s="4"/>
       <c r="C122" s="8"/>
       <c r="D122" s="8"/>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="3"/>
       <c r="B123" s="4"/>
       <c r="C123" s="8"/>
       <c r="D123" s="8"/>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="3"/>
       <c r="B124" s="4"/>
       <c r="C124" s="8"/>
       <c r="D124" s="8"/>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="3"/>
       <c r="B125" s="4"/>
       <c r="C125" s="8"/>
       <c r="D125" s="8"/>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="3"/>
       <c r="B126" s="4"/>
       <c r="C126" s="8"/>
       <c r="D126" s="8"/>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="3"/>
       <c r="B127" s="4"/>
       <c r="C127" s="8"/>
       <c r="D127" s="8"/>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="3"/>
       <c r="B128" s="4"/>
       <c r="C128" s="8"/>
       <c r="D128" s="8"/>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="3"/>
       <c r="B129" s="4"/>
       <c r="C129" s="8"/>
       <c r="D129" s="8"/>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="3"/>
       <c r="B130" s="4"/>
       <c r="C130" s="8"/>
       <c r="D130" s="8"/>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="3"/>
       <c r="B131" s="4"/>
       <c r="C131" s="8"/>
       <c r="D131" s="8"/>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="3"/>
       <c r="B132" s="4"/>
       <c r="C132" s="8"/>
       <c r="D132" s="8"/>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="3"/>
       <c r="B133" s="4"/>
       <c r="C133" s="8"/>
       <c r="D133" s="8"/>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="3"/>
       <c r="B134" s="4"/>
       <c r="C134" s="8"/>
       <c r="D134" s="8"/>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="3"/>
       <c r="B135" s="4"/>
       <c r="C135" s="8"/>
       <c r="D135" s="8"/>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="3"/>
       <c r="B136" s="4"/>
       <c r="C136" s="8"/>
       <c r="D136" s="8"/>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="3"/>
       <c r="B137" s="4"/>
       <c r="C137" s="8"/>
       <c r="D137" s="8"/>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="3"/>
       <c r="B138" s="4"/>
       <c r="C138" s="8"/>
       <c r="D138" s="8"/>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="3"/>
       <c r="B139" s="4"/>
       <c r="C139" s="8"/>
       <c r="D139" s="8"/>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="3"/>
       <c r="B140" s="4"/>
       <c r="C140" s="8"/>
       <c r="D140" s="8"/>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="3"/>
       <c r="B141" s="4"/>
       <c r="C141" s="8"/>
       <c r="D141" s="8"/>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="9"/>
       <c r="B142" s="4"/>
       <c r="C142" s="8"/>
       <c r="D142" s="8"/>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="9"/>
       <c r="B143" s="4"/>
       <c r="C143" s="8"/>
       <c r="D143" s="8"/>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="9"/>
       <c r="B144" s="4"/>
       <c r="C144" s="8"/>
       <c r="D144" s="8"/>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="9"/>
       <c r="B145" s="4"/>
       <c r="C145" s="8"/>
       <c r="D145" s="8"/>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="9"/>
       <c r="B146" s="4"/>
       <c r="C146" s="8"/>
       <c r="D146" s="8"/>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="9"/>
       <c r="B147" s="4"/>
       <c r="C147" s="8"/>
       <c r="D147" s="8"/>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="9"/>
       <c r="B148" s="4"/>
       <c r="C148" s="8"/>
       <c r="D148" s="8"/>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="9"/>
       <c r="B149" s="4"/>
       <c r="C149" s="8"/>
       <c r="D149" s="8"/>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="9"/>
       <c r="B150" s="4"/>
       <c r="C150" s="8"/>
       <c r="D150" s="8"/>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="9"/>
       <c r="B151" s="4"/>
       <c r="C151" s="8"/>
       <c r="D151" s="8"/>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="3"/>
       <c r="B152" s="4"/>
       <c r="C152" s="8"/>
       <c r="D152" s="8"/>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="3"/>
       <c r="B153" s="4"/>
       <c r="C153" s="8"/>
       <c r="D153" s="8"/>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="3"/>
       <c r="B154" s="4"/>
       <c r="C154" s="8"/>
       <c r="D154" s="8"/>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="3"/>
       <c r="B155" s="4"/>
       <c r="C155" s="8"/>
       <c r="D155" s="8"/>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" s="3"/>
       <c r="B156" s="4"/>
       <c r="C156" s="8"/>
       <c r="D156" s="8"/>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="4"/>
       <c r="B157" s="5"/>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" s="4"/>
       <c r="B158" s="5"/>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="4"/>
       <c r="B159" s="5"/>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="4"/>
       <c r="B160" s="5"/>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" s="4"/>
       <c r="B161" s="5"/>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" s="4"/>
       <c r="B162" s="5"/>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" s="4"/>
       <c r="B163" s="5"/>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" s="4"/>
       <c r="B164" s="5"/>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" s="4"/>
       <c r="B165" s="5"/>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" s="4"/>
       <c r="B166" s="5"/>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" s="4"/>
       <c r="B167" s="5"/>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" s="4"/>
       <c r="B168" s="5"/>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" s="4"/>
       <c r="B169" s="5"/>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" s="4"/>
       <c r="B170" s="5"/>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" s="4"/>
       <c r="B171" s="5"/>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" s="4"/>
       <c r="B172" s="5"/>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" s="4"/>
       <c r="B173" s="5"/>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" s="4"/>
       <c r="B174" s="5"/>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" s="4"/>
       <c r="B175" s="5"/>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" s="4"/>
       <c r="B176" s="5"/>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" s="4"/>
       <c r="B177" s="5"/>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" s="4"/>
       <c r="B178" s="5"/>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" s="4"/>
       <c r="B179" s="5"/>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" s="4"/>
       <c r="B180" s="5"/>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" s="4"/>
       <c r="B181" s="5"/>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" s="4"/>
       <c r="B182" s="5"/>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" s="4"/>
       <c r="B183" s="5"/>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" s="4"/>
       <c r="B184" s="5"/>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" s="4"/>
       <c r="B185" s="5"/>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" s="4"/>
       <c r="B186" s="5"/>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" s="4"/>
       <c r="B187" s="5"/>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" s="4"/>
       <c r="B188" s="5"/>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" s="4"/>
       <c r="B189" s="5"/>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" s="4"/>
       <c r="B190" s="5"/>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" s="4"/>
       <c r="B191" s="5"/>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" s="4"/>
       <c r="B192" s="5"/>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" s="4"/>
       <c r="B193" s="5"/>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" s="4"/>
       <c r="B194" s="5"/>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" s="4"/>
       <c r="B195" s="5"/>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" s="4"/>
       <c r="B196" s="5"/>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" s="4"/>
       <c r="B197" s="5"/>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" s="4"/>
       <c r="B198" s="5"/>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" s="4"/>
       <c r="B199" s="5"/>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" s="4"/>
       <c r="B200" s="5"/>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" s="4"/>
       <c r="B201" s="5"/>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" s="4"/>
       <c r="B202" s="5"/>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" s="4"/>
       <c r="B203" s="5"/>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" s="4"/>
       <c r="B204" s="5"/>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" s="4"/>
       <c r="B205" s="5"/>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" s="4"/>
       <c r="B206" s="5"/>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" s="4"/>
       <c r="B207" s="5"/>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" s="4"/>
       <c r="B208" s="5"/>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" s="4"/>
       <c r="B209" s="5"/>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" s="4"/>
       <c r="B210" s="5"/>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" s="4"/>
       <c r="B211" s="5"/>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" s="4"/>
       <c r="B212" s="5"/>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" s="4"/>
       <c r="B213" s="5"/>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" s="4"/>
       <c r="B214" s="5"/>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" s="4"/>
       <c r="B215" s="5"/>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" s="4"/>
       <c r="B216" s="5"/>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" s="4"/>
       <c r="B217" s="5"/>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" s="4"/>
       <c r="B218" s="5"/>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" s="4"/>
       <c r="B219" s="5"/>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" s="4"/>
       <c r="B220" s="5"/>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" s="4"/>
       <c r="B221" s="5"/>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" s="4"/>
       <c r="B222" s="5"/>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" s="4"/>
       <c r="B223" s="5"/>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" s="4"/>
       <c r="B224" s="5"/>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" s="4"/>
       <c r="B225" s="5"/>
     </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" s="4"/>
       <c r="B226" s="5"/>
     </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" s="4"/>
       <c r="B227" s="5"/>
     </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" s="4"/>
       <c r="B228" s="5"/>
     </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" s="4"/>
       <c r="B229" s="5"/>
     </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" s="4"/>
       <c r="B230" s="5"/>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" s="4"/>
       <c r="B231" s="5"/>
     </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" s="4"/>
       <c r="B232" s="5"/>
     </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" s="4"/>
       <c r="B233" s="5"/>
     </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" s="4"/>
       <c r="B234" s="5"/>
     </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" s="4"/>
       <c r="B235" s="5"/>
     </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" s="4"/>
       <c r="B236" s="5"/>
     </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" s="4"/>
       <c r="B237" s="5"/>
     </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" s="4"/>
       <c r="B238" s="5"/>
     </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" s="4"/>
       <c r="B239" s="5"/>
     </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" s="3"/>
       <c r="B240" s="5"/>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" s="3"/>
       <c r="B241" s="5"/>
     </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" s="3"/>
       <c r="B242" s="5"/>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" s="3"/>
       <c r="B243" s="5"/>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" s="3"/>
       <c r="B244" s="5"/>
     </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" s="3"/>
       <c r="B245" s="5"/>
     </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" s="3"/>
       <c r="B246" s="5"/>
     </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" s="3"/>
       <c r="B247" s="5"/>
     </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248" s="3"/>
       <c r="B248" s="5"/>
     </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" s="3"/>
       <c r="B249" s="5"/>
     </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250" s="3"/>
       <c r="B250" s="5"/>
     </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251" s="3"/>
       <c r="B251" s="5"/>
     </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A252" s="3"/>
       <c r="B252" s="5"/>
     </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253" s="3"/>
       <c r="B253" s="5"/>
     </row>
@@ -3950,18 +3981,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -4202,6 +4221,18 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -4212,17 +4243,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D9CBEFE-8C4C-4054-8E02-CA457E93B4C8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
-    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F0D7176-14CB-4F63-BBB4-5E9CDAB9112D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4241,6 +4261,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D9CBEFE-8C4C-4054-8E02-CA457E93B4C8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
+    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C05FF1B-7508-40EF-8319-E993EA07F007}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
added category 4 for SMOKE_ST to DD
</commit_message>
<xml_diff>
--- a/rmonize/data_dictionary/DD_KORA_S3_P1.xlsx
+++ b/rmonize/data_dictionary/DD_KORA_S3_P1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\rmonize\data_dictionary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\NFDI4Health\TA5\Pilotprojekte\Harmonisierung\HarmonizR\use-cases-harmonisation\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6648FBF3-3346-4A94-85DF-3FF356A948E1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C3F797E-346B-4082-A741-94C905E862EC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22320" windowHeight="11940" xr2:uid="{1200B70D-B446-4CDA-99A8-3FD394D791D2}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="22320" windowHeight="11940" activeTab="1" xr2:uid="{1200B70D-B446-4CDA-99A8-3FD394D791D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="220">
   <si>
     <t>index</t>
   </si>
@@ -683,6 +683,9 @@
   </si>
   <si>
     <t>energy</t>
+  </si>
+  <si>
+    <t>unknown</t>
   </si>
 </sst>
 </file>
@@ -1091,19 +1094,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08A73012-5CAD-43B9-A281-79101DF4E1E0}">
   <dimension ref="A1:F102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" style="9" customWidth="1"/>
-    <col min="2" max="2" width="20.44140625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="39.88671875" style="9" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" style="9"/>
+    <col min="1" max="1" width="9.42578125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="39.85546875" style="9" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1117,7 +1120,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
         <v>1</v>
       </c>
@@ -1131,7 +1134,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <v>2</v>
       </c>
@@ -1145,7 +1148,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>3</v>
       </c>
@@ -1159,7 +1162,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>4</v>
       </c>
@@ -1173,7 +1176,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>5</v>
       </c>
@@ -1187,7 +1190,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>6</v>
       </c>
@@ -1201,7 +1204,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>7</v>
       </c>
@@ -1215,7 +1218,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>8</v>
       </c>
@@ -1229,7 +1232,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>9</v>
       </c>
@@ -1243,7 +1246,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>10</v>
       </c>
@@ -1257,7 +1260,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>11</v>
       </c>
@@ -1271,7 +1274,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>12</v>
       </c>
@@ -1285,7 +1288,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>13</v>
       </c>
@@ -1299,7 +1302,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>14</v>
       </c>
@@ -1313,7 +1316,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>15</v>
       </c>
@@ -1327,7 +1330,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>16</v>
       </c>
@@ -1341,7 +1344,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>17</v>
       </c>
@@ -1355,7 +1358,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
         <v>18</v>
       </c>
@@ -1369,7 +1372,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
         <v>19</v>
       </c>
@@ -1383,7 +1386,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
         <v>20</v>
       </c>
@@ -1397,7 +1400,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
         <v>21</v>
       </c>
@@ -1411,7 +1414,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
         <v>22</v>
       </c>
@@ -1425,7 +1428,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
         <v>23</v>
       </c>
@@ -1439,7 +1442,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
         <v>24</v>
       </c>
@@ -1453,7 +1456,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="9">
         <v>25</v>
       </c>
@@ -1467,7 +1470,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="9">
         <v>26</v>
       </c>
@@ -1481,7 +1484,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="9">
         <v>27</v>
       </c>
@@ -1495,7 +1498,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="9">
         <v>28</v>
       </c>
@@ -1509,7 +1512,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="9">
         <v>29</v>
       </c>
@@ -1523,7 +1526,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="9">
         <v>30</v>
       </c>
@@ -1537,7 +1540,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="9">
         <v>31</v>
       </c>
@@ -1551,7 +1554,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="9">
         <v>32</v>
       </c>
@@ -1565,7 +1568,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="9">
         <v>33</v>
       </c>
@@ -1579,7 +1582,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="9">
         <v>34</v>
       </c>
@@ -1593,7 +1596,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="9">
         <v>35</v>
       </c>
@@ -1607,7 +1610,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="9">
         <v>36</v>
       </c>
@@ -1621,7 +1624,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="9">
         <v>37</v>
       </c>
@@ -1635,7 +1638,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="9">
         <v>38</v>
       </c>
@@ -1649,7 +1652,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="9">
         <v>39</v>
       </c>
@@ -1663,7 +1666,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="9">
         <v>40</v>
       </c>
@@ -1677,7 +1680,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="9">
         <v>41</v>
       </c>
@@ -1691,7 +1694,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="9">
         <v>42</v>
       </c>
@@ -1705,7 +1708,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="9">
         <v>43</v>
       </c>
@@ -1719,7 +1722,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="9">
         <v>44</v>
       </c>
@@ -1733,7 +1736,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="9">
         <v>45</v>
       </c>
@@ -1747,7 +1750,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="9">
         <v>46</v>
       </c>
@@ -1761,7 +1764,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="9">
         <v>47</v>
       </c>
@@ -1775,7 +1778,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="9">
         <v>48</v>
       </c>
@@ -1789,7 +1792,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="9">
         <v>49</v>
       </c>
@@ -1803,7 +1806,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="9">
         <v>50</v>
       </c>
@@ -1817,7 +1820,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="9">
         <v>51</v>
       </c>
@@ -1831,7 +1834,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="9">
         <v>52</v>
       </c>
@@ -1845,7 +1848,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="9">
         <v>53</v>
       </c>
@@ -1859,7 +1862,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="9">
         <v>54</v>
       </c>
@@ -1873,7 +1876,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="9">
         <v>55</v>
       </c>
@@ -1887,7 +1890,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="9">
         <v>56</v>
       </c>
@@ -1901,7 +1904,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="9">
         <v>57</v>
       </c>
@@ -1915,7 +1918,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="9">
         <v>58</v>
       </c>
@@ -1929,7 +1932,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="9">
         <v>59</v>
       </c>
@@ -1943,7 +1946,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="9">
         <v>60</v>
       </c>
@@ -1957,7 +1960,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="9">
         <v>61</v>
       </c>
@@ -1971,7 +1974,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="9">
         <v>62</v>
       </c>
@@ -1985,7 +1988,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="9">
         <v>63</v>
       </c>
@@ -1999,7 +2002,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="9">
         <v>64</v>
       </c>
@@ -2013,7 +2016,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="9">
         <v>65</v>
       </c>
@@ -2027,7 +2030,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="9">
         <v>66</v>
       </c>
@@ -2041,7 +2044,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="9">
         <v>67</v>
       </c>
@@ -2055,7 +2058,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="9">
         <v>68</v>
       </c>
@@ -2069,7 +2072,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="9">
         <v>69</v>
       </c>
@@ -2083,7 +2086,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="9">
         <v>70</v>
       </c>
@@ -2097,7 +2100,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="9">
         <v>71</v>
       </c>
@@ -2111,7 +2114,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="9">
         <v>72</v>
       </c>
@@ -2125,7 +2128,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="9">
         <v>73</v>
       </c>
@@ -2139,7 +2142,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="9">
         <v>74</v>
       </c>
@@ -2153,7 +2156,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="9">
         <v>75</v>
       </c>
@@ -2167,7 +2170,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="9">
         <v>76</v>
       </c>
@@ -2181,7 +2184,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="9">
         <v>77</v>
       </c>
@@ -2195,7 +2198,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="9">
         <v>78</v>
       </c>
@@ -2209,7 +2212,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="9">
         <v>79</v>
       </c>
@@ -2223,7 +2226,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="9">
         <v>80</v>
       </c>
@@ -2237,7 +2240,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="9">
         <v>81</v>
       </c>
@@ -2251,7 +2254,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="9">
         <v>82</v>
       </c>
@@ -2265,7 +2268,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="9">
         <v>83</v>
       </c>
@@ -2279,7 +2282,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="9">
         <v>84</v>
       </c>
@@ -2293,7 +2296,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="9">
         <v>85</v>
       </c>
@@ -2307,7 +2310,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="9">
         <v>86</v>
       </c>
@@ -2321,7 +2324,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="9">
         <v>87</v>
       </c>
@@ -2335,7 +2338,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="9">
         <v>88</v>
       </c>
@@ -2349,7 +2352,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="9">
         <v>89</v>
       </c>
@@ -2363,7 +2366,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="9">
         <v>90</v>
       </c>
@@ -2377,7 +2380,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="9">
         <v>91</v>
       </c>
@@ -2391,7 +2394,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="9">
         <v>92</v>
       </c>
@@ -2408,7 +2411,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="9">
         <v>93</v>
       </c>
@@ -2422,7 +2425,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="9">
         <v>94</v>
       </c>
@@ -2436,7 +2439,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="9">
         <v>95</v>
       </c>
@@ -2450,7 +2453,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="9">
         <v>96</v>
       </c>
@@ -2464,7 +2467,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="9">
         <v>97</v>
       </c>
@@ -2478,7 +2481,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="9">
         <v>98</v>
       </c>
@@ -2492,7 +2495,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="9">
         <v>99</v>
       </c>
@@ -2506,7 +2509,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="9">
         <v>100</v>
       </c>
@@ -2520,7 +2523,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="9">
         <v>101</v>
       </c>
@@ -2544,16 +2547,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7CFBFAA-22DC-428C-A718-7E0BADD40216}">
   <dimension ref="A1:G249"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" customWidth="1"/>
-    <col min="2" max="2" width="7.109375" customWidth="1"/>
-    <col min="3" max="3" width="34.44140625" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" customWidth="1"/>
+    <col min="3" max="3" width="34.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>204</v>
       </c>
@@ -2568,7 +2573,7 @@
       </c>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>5</v>
       </c>
@@ -2582,7 +2587,7 @@
       <c r="F2" s="6"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>10</v>
       </c>
@@ -2596,7 +2601,7 @@
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
     </row>
-    <row r="4" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>10</v>
       </c>
@@ -2610,7 +2615,7 @@
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
     </row>
-    <row r="5" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>10</v>
       </c>
@@ -2624,7 +2629,7 @@
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
     </row>
-    <row r="6" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>10</v>
       </c>
@@ -2638,7 +2643,7 @@
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
     </row>
-    <row r="7" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>12</v>
       </c>
@@ -2652,7 +2657,7 @@
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
     </row>
-    <row r="8" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
@@ -2666,7 +2671,7 @@
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
     </row>
-    <row r="9" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>12</v>
       </c>
@@ -2677,1249 +2682,1255 @@
         <v>210</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="2"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="8"/>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="12">
+        <v>4</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>219</v>
+      </c>
       <c r="D10" s="8"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="4"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="4"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="4"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="4"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="4"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="4"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="4"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="4"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="4"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="4"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="4"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="4"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="4"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="4"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="4"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="4"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="4"/>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="4"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="4"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="4"/>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="4"/>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="4"/>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="4"/>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="4"/>
       <c r="C34" s="8"/>
       <c r="D34" s="8"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="4"/>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="4"/>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="4"/>
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="4"/>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
       <c r="B39" s="4"/>
       <c r="C39" s="8"/>
       <c r="D39" s="8"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="4"/>
       <c r="C40" s="8"/>
       <c r="D40" s="8"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
       <c r="B41" s="4"/>
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="4"/>
       <c r="C42" s="8"/>
       <c r="D42" s="8"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
       <c r="B43" s="4"/>
       <c r="C43" s="8"/>
       <c r="D43" s="8"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
       <c r="B44" s="4"/>
       <c r="C44" s="8"/>
       <c r="D44" s="8"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
       <c r="B45" s="4"/>
       <c r="C45" s="8"/>
       <c r="D45" s="8"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
       <c r="B46" s="4"/>
       <c r="C46" s="8"/>
       <c r="D46" s="8"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
       <c r="B47" s="4"/>
       <c r="C47" s="8"/>
       <c r="D47" s="8"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" s="4"/>
       <c r="C48" s="8"/>
       <c r="D48" s="8"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
       <c r="B49" s="4"/>
       <c r="C49" s="8"/>
       <c r="D49" s="8"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
       <c r="B50" s="4"/>
       <c r="C50" s="8"/>
       <c r="D50" s="8"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
       <c r="B51" s="4"/>
       <c r="C51" s="8"/>
       <c r="D51" s="8"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
       <c r="B52" s="4"/>
       <c r="C52" s="8"/>
       <c r="D52" s="8"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="3"/>
       <c r="B53" s="4"/>
       <c r="C53" s="8"/>
       <c r="D53" s="8"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
       <c r="B54" s="4"/>
       <c r="C54" s="8"/>
       <c r="D54" s="8"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="3"/>
       <c r="B55" s="4"/>
       <c r="C55" s="8"/>
       <c r="D55" s="8"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
       <c r="B56" s="4"/>
       <c r="C56" s="8"/>
       <c r="D56" s="8"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="3"/>
       <c r="B57" s="4"/>
       <c r="C57" s="8"/>
       <c r="D57" s="8"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="3"/>
       <c r="B58" s="4"/>
       <c r="C58" s="8"/>
       <c r="D58" s="8"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="3"/>
       <c r="B59" s="4"/>
       <c r="C59" s="8"/>
       <c r="D59" s="8"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="3"/>
       <c r="B60" s="4"/>
       <c r="C60" s="8"/>
       <c r="D60" s="8"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="3"/>
       <c r="B61" s="4"/>
       <c r="C61" s="8"/>
       <c r="D61" s="8"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
       <c r="B62" s="4"/>
       <c r="C62" s="8"/>
       <c r="D62" s="8"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="3"/>
       <c r="B63" s="4"/>
       <c r="C63" s="8"/>
       <c r="D63" s="8"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="3"/>
       <c r="B64" s="4"/>
       <c r="C64" s="8"/>
       <c r="D64" s="8"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="3"/>
       <c r="B65" s="4"/>
       <c r="C65" s="8"/>
       <c r="D65" s="8"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="3"/>
       <c r="B66" s="4"/>
       <c r="C66" s="8"/>
       <c r="D66" s="8"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="3"/>
       <c r="B67" s="4"/>
       <c r="C67" s="8"/>
       <c r="D67" s="8"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
       <c r="B68" s="4"/>
       <c r="C68" s="8"/>
       <c r="D68" s="8"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="3"/>
       <c r="B69" s="4"/>
       <c r="C69" s="8"/>
       <c r="D69" s="8"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="3"/>
       <c r="B70" s="4"/>
       <c r="C70" s="8"/>
       <c r="D70" s="8"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="3"/>
       <c r="B71" s="4"/>
       <c r="C71" s="8"/>
       <c r="D71" s="8"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="3"/>
       <c r="B72" s="4"/>
       <c r="C72" s="8"/>
       <c r="D72" s="8"/>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="3"/>
       <c r="B73" s="4"/>
       <c r="C73" s="8"/>
       <c r="D73" s="8"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="3"/>
       <c r="B74" s="4"/>
       <c r="C74" s="8"/>
       <c r="D74" s="8"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="3"/>
       <c r="B75" s="4"/>
       <c r="C75" s="8"/>
       <c r="D75" s="8"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="3"/>
       <c r="B76" s="4"/>
       <c r="C76" s="8"/>
       <c r="D76" s="8"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="3"/>
       <c r="B77" s="4"/>
       <c r="C77" s="8"/>
       <c r="D77" s="8"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="3"/>
       <c r="B78" s="4"/>
       <c r="C78" s="8"/>
       <c r="D78" s="8"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="3"/>
       <c r="B79" s="4"/>
       <c r="C79" s="8"/>
       <c r="D79" s="8"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="3"/>
       <c r="B80" s="4"/>
       <c r="C80" s="8"/>
       <c r="D80" s="8"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="3"/>
       <c r="B81" s="4"/>
       <c r="C81" s="8"/>
       <c r="D81" s="8"/>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="3"/>
       <c r="B82" s="4"/>
       <c r="C82" s="8"/>
       <c r="D82" s="8"/>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="3"/>
       <c r="B83" s="4"/>
       <c r="C83" s="8"/>
       <c r="D83" s="8"/>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="3"/>
       <c r="B84" s="4"/>
       <c r="C84" s="8"/>
       <c r="D84" s="8"/>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="3"/>
       <c r="B85" s="4"/>
       <c r="C85" s="8"/>
       <c r="D85" s="8"/>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="3"/>
       <c r="B86" s="4"/>
       <c r="C86" s="8"/>
       <c r="D86" s="8"/>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="3"/>
       <c r="B87" s="4"/>
       <c r="C87" s="8"/>
       <c r="D87" s="8"/>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="3"/>
       <c r="B88" s="4"/>
       <c r="C88" s="8"/>
       <c r="D88" s="8"/>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="3"/>
       <c r="B89" s="4"/>
       <c r="C89" s="8"/>
       <c r="D89" s="8"/>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="3"/>
       <c r="B90" s="4"/>
       <c r="C90" s="8"/>
       <c r="D90" s="8"/>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="3"/>
       <c r="B91" s="4"/>
       <c r="C91" s="8"/>
       <c r="D91" s="8"/>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="3"/>
       <c r="B92" s="4"/>
       <c r="C92" s="8"/>
       <c r="D92" s="8"/>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="3"/>
       <c r="B93" s="4"/>
       <c r="C93" s="8"/>
       <c r="D93" s="8"/>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="3"/>
       <c r="B94" s="4"/>
       <c r="C94" s="8"/>
       <c r="D94" s="8"/>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="3"/>
       <c r="B95" s="4"/>
       <c r="C95" s="8"/>
       <c r="D95" s="8"/>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="3"/>
       <c r="B96" s="4"/>
       <c r="C96" s="8"/>
       <c r="D96" s="8"/>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="3"/>
       <c r="B97" s="4"/>
       <c r="C97" s="8"/>
       <c r="D97" s="8"/>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="3"/>
       <c r="B98" s="4"/>
       <c r="C98" s="8"/>
       <c r="D98" s="8"/>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="3"/>
       <c r="B99" s="4"/>
       <c r="C99" s="8"/>
       <c r="D99" s="8"/>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="3"/>
       <c r="B100" s="4"/>
       <c r="C100" s="8"/>
       <c r="D100" s="8"/>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="3"/>
       <c r="B101" s="4"/>
       <c r="C101" s="8"/>
       <c r="D101" s="8"/>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="3"/>
       <c r="B102" s="4"/>
       <c r="C102" s="8"/>
       <c r="D102" s="8"/>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="3"/>
       <c r="B103" s="4"/>
       <c r="C103" s="8"/>
       <c r="D103" s="8"/>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="3"/>
       <c r="B104" s="4"/>
       <c r="C104" s="8"/>
       <c r="D104" s="8"/>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="3"/>
       <c r="B105" s="4"/>
       <c r="C105" s="8"/>
       <c r="D105" s="8"/>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="3"/>
       <c r="B106" s="4"/>
       <c r="C106" s="8"/>
       <c r="D106" s="8"/>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="3"/>
       <c r="B107" s="4"/>
       <c r="C107" s="8"/>
       <c r="D107" s="8"/>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="3"/>
       <c r="B108" s="4"/>
       <c r="C108" s="8"/>
       <c r="D108" s="8"/>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="3"/>
       <c r="B109" s="4"/>
       <c r="C109" s="8"/>
       <c r="D109" s="8"/>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="3"/>
       <c r="B110" s="4"/>
       <c r="C110" s="8"/>
       <c r="D110" s="8"/>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="3"/>
       <c r="B111" s="4"/>
       <c r="C111" s="8"/>
       <c r="D111" s="8"/>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="3"/>
       <c r="B112" s="4"/>
       <c r="C112" s="8"/>
       <c r="D112" s="8"/>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="3"/>
       <c r="B113" s="4"/>
       <c r="C113" s="8"/>
       <c r="D113" s="8"/>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="3"/>
       <c r="B114" s="4"/>
       <c r="C114" s="8"/>
       <c r="D114" s="8"/>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="3"/>
       <c r="B115" s="4"/>
       <c r="C115" s="8"/>
       <c r="D115" s="8"/>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="3"/>
       <c r="B116" s="4"/>
       <c r="C116" s="8"/>
       <c r="D116" s="8"/>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="3"/>
       <c r="B117" s="4"/>
       <c r="C117" s="8"/>
       <c r="D117" s="8"/>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="3"/>
       <c r="B118" s="4"/>
       <c r="C118" s="8"/>
       <c r="D118" s="8"/>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="3"/>
       <c r="B119" s="4"/>
       <c r="C119" s="8"/>
       <c r="D119" s="8"/>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="3"/>
       <c r="B120" s="4"/>
       <c r="C120" s="8"/>
       <c r="D120" s="8"/>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="3"/>
       <c r="B121" s="4"/>
       <c r="C121" s="8"/>
       <c r="D121" s="8"/>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="3"/>
       <c r="B122" s="4"/>
       <c r="C122" s="8"/>
       <c r="D122" s="8"/>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="3"/>
       <c r="B123" s="4"/>
       <c r="C123" s="8"/>
       <c r="D123" s="8"/>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="3"/>
       <c r="B124" s="4"/>
       <c r="C124" s="8"/>
       <c r="D124" s="8"/>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="3"/>
       <c r="B125" s="4"/>
       <c r="C125" s="8"/>
       <c r="D125" s="8"/>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="3"/>
       <c r="B126" s="4"/>
       <c r="C126" s="8"/>
       <c r="D126" s="8"/>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="3"/>
       <c r="B127" s="4"/>
       <c r="C127" s="8"/>
       <c r="D127" s="8"/>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="3"/>
       <c r="B128" s="4"/>
       <c r="C128" s="8"/>
       <c r="D128" s="8"/>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="3"/>
       <c r="B129" s="4"/>
       <c r="C129" s="8"/>
       <c r="D129" s="8"/>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="3"/>
       <c r="B130" s="4"/>
       <c r="C130" s="8"/>
       <c r="D130" s="8"/>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="3"/>
       <c r="B131" s="4"/>
       <c r="C131" s="8"/>
       <c r="D131" s="8"/>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="3"/>
       <c r="B132" s="4"/>
       <c r="C132" s="8"/>
       <c r="D132" s="8"/>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="3"/>
       <c r="B133" s="4"/>
       <c r="C133" s="8"/>
       <c r="D133" s="8"/>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="3"/>
       <c r="B134" s="4"/>
       <c r="C134" s="8"/>
       <c r="D134" s="8"/>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="3"/>
       <c r="B135" s="4"/>
       <c r="C135" s="8"/>
       <c r="D135" s="8"/>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="3"/>
       <c r="B136" s="4"/>
       <c r="C136" s="8"/>
       <c r="D136" s="8"/>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="3"/>
       <c r="B137" s="4"/>
       <c r="C137" s="8"/>
       <c r="D137" s="8"/>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="9"/>
       <c r="B138" s="4"/>
       <c r="C138" s="8"/>
       <c r="D138" s="8"/>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="9"/>
       <c r="B139" s="4"/>
       <c r="C139" s="8"/>
       <c r="D139" s="8"/>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="9"/>
       <c r="B140" s="4"/>
       <c r="C140" s="8"/>
       <c r="D140" s="8"/>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="9"/>
       <c r="B141" s="4"/>
       <c r="C141" s="8"/>
       <c r="D141" s="8"/>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="9"/>
       <c r="B142" s="4"/>
       <c r="C142" s="8"/>
       <c r="D142" s="8"/>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="9"/>
       <c r="B143" s="4"/>
       <c r="C143" s="8"/>
       <c r="D143" s="8"/>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="9"/>
       <c r="B144" s="4"/>
       <c r="C144" s="8"/>
       <c r="D144" s="8"/>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="9"/>
       <c r="B145" s="4"/>
       <c r="C145" s="8"/>
       <c r="D145" s="8"/>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="9"/>
       <c r="B146" s="4"/>
       <c r="C146" s="8"/>
       <c r="D146" s="8"/>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="9"/>
       <c r="B147" s="4"/>
       <c r="C147" s="8"/>
       <c r="D147" s="8"/>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="3"/>
       <c r="B148" s="4"/>
       <c r="C148" s="8"/>
       <c r="D148" s="8"/>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="3"/>
       <c r="B149" s="4"/>
       <c r="C149" s="8"/>
       <c r="D149" s="8"/>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="3"/>
       <c r="B150" s="4"/>
       <c r="C150" s="8"/>
       <c r="D150" s="8"/>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="3"/>
       <c r="B151" s="4"/>
       <c r="C151" s="8"/>
       <c r="D151" s="8"/>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="3"/>
       <c r="B152" s="4"/>
       <c r="C152" s="8"/>
       <c r="D152" s="8"/>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="4"/>
       <c r="B153" s="5"/>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="4"/>
       <c r="B154" s="5"/>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="4"/>
       <c r="B155" s="5"/>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" s="4"/>
       <c r="B156" s="5"/>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="4"/>
       <c r="B157" s="5"/>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" s="4"/>
       <c r="B158" s="5"/>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="4"/>
       <c r="B159" s="5"/>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="4"/>
       <c r="B160" s="5"/>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" s="4"/>
       <c r="B161" s="5"/>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" s="4"/>
       <c r="B162" s="5"/>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" s="4"/>
       <c r="B163" s="5"/>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" s="4"/>
       <c r="B164" s="5"/>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" s="4"/>
       <c r="B165" s="5"/>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" s="4"/>
       <c r="B166" s="5"/>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" s="4"/>
       <c r="B167" s="5"/>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" s="4"/>
       <c r="B168" s="5"/>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" s="4"/>
       <c r="B169" s="5"/>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" s="4"/>
       <c r="B170" s="5"/>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" s="4"/>
       <c r="B171" s="5"/>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" s="4"/>
       <c r="B172" s="5"/>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" s="4"/>
       <c r="B173" s="5"/>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" s="4"/>
       <c r="B174" s="5"/>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" s="4"/>
       <c r="B175" s="5"/>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" s="4"/>
       <c r="B176" s="5"/>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" s="4"/>
       <c r="B177" s="5"/>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" s="4"/>
       <c r="B178" s="5"/>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" s="4"/>
       <c r="B179" s="5"/>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" s="4"/>
       <c r="B180" s="5"/>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" s="4"/>
       <c r="B181" s="5"/>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" s="4"/>
       <c r="B182" s="5"/>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" s="4"/>
       <c r="B183" s="5"/>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" s="4"/>
       <c r="B184" s="5"/>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" s="4"/>
       <c r="B185" s="5"/>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" s="4"/>
       <c r="B186" s="5"/>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" s="4"/>
       <c r="B187" s="5"/>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" s="4"/>
       <c r="B188" s="5"/>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" s="4"/>
       <c r="B189" s="5"/>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" s="4"/>
       <c r="B190" s="5"/>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" s="4"/>
       <c r="B191" s="5"/>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" s="4"/>
       <c r="B192" s="5"/>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" s="4"/>
       <c r="B193" s="5"/>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" s="4"/>
       <c r="B194" s="5"/>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" s="4"/>
       <c r="B195" s="5"/>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" s="4"/>
       <c r="B196" s="5"/>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" s="4"/>
       <c r="B197" s="5"/>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" s="4"/>
       <c r="B198" s="5"/>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" s="4"/>
       <c r="B199" s="5"/>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" s="4"/>
       <c r="B200" s="5"/>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" s="4"/>
       <c r="B201" s="5"/>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" s="4"/>
       <c r="B202" s="5"/>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" s="4"/>
       <c r="B203" s="5"/>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" s="4"/>
       <c r="B204" s="5"/>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" s="4"/>
       <c r="B205" s="5"/>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" s="4"/>
       <c r="B206" s="5"/>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" s="4"/>
       <c r="B207" s="5"/>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" s="4"/>
       <c r="B208" s="5"/>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" s="4"/>
       <c r="B209" s="5"/>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" s="4"/>
       <c r="B210" s="5"/>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" s="4"/>
       <c r="B211" s="5"/>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" s="4"/>
       <c r="B212" s="5"/>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" s="4"/>
       <c r="B213" s="5"/>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" s="4"/>
       <c r="B214" s="5"/>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" s="4"/>
       <c r="B215" s="5"/>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" s="4"/>
       <c r="B216" s="5"/>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" s="4"/>
       <c r="B217" s="5"/>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" s="4"/>
       <c r="B218" s="5"/>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" s="4"/>
       <c r="B219" s="5"/>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" s="4"/>
       <c r="B220" s="5"/>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" s="4"/>
       <c r="B221" s="5"/>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" s="4"/>
       <c r="B222" s="5"/>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" s="4"/>
       <c r="B223" s="5"/>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" s="4"/>
       <c r="B224" s="5"/>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" s="4"/>
       <c r="B225" s="5"/>
     </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" s="4"/>
       <c r="B226" s="5"/>
     </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" s="4"/>
       <c r="B227" s="5"/>
     </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" s="4"/>
       <c r="B228" s="5"/>
     </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" s="4"/>
       <c r="B229" s="5"/>
     </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" s="4"/>
       <c r="B230" s="5"/>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" s="4"/>
       <c r="B231" s="5"/>
     </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" s="4"/>
       <c r="B232" s="5"/>
     </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" s="4"/>
       <c r="B233" s="5"/>
     </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" s="4"/>
       <c r="B234" s="5"/>
     </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" s="4"/>
       <c r="B235" s="5"/>
     </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" s="3"/>
       <c r="B236" s="5"/>
     </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" s="3"/>
       <c r="B237" s="5"/>
     </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" s="3"/>
       <c r="B238" s="5"/>
     </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" s="3"/>
       <c r="B239" s="5"/>
     </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" s="3"/>
       <c r="B240" s="5"/>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" s="3"/>
       <c r="B241" s="5"/>
     </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" s="3"/>
       <c r="B242" s="5"/>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" s="3"/>
       <c r="B243" s="5"/>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" s="3"/>
       <c r="B244" s="5"/>
     </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" s="3"/>
       <c r="B245" s="5"/>
     </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" s="3"/>
       <c r="B246" s="5"/>
     </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" s="3"/>
       <c r="B247" s="5"/>
     </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248" s="3"/>
       <c r="B248" s="5"/>
     </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" s="3"/>
       <c r="B249" s="5"/>
     </row>
@@ -3939,6 +3950,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -4179,18 +4202,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C05FF1B-7508-40EF-8319-E993EA07F007}">
   <ds:schemaRefs>
@@ -4200,6 +4211,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D9CBEFE-8C4C-4054-8E02-CA457E93B4C8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F0D7176-14CB-4F63-BBB4-5E9CDAB9112D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4216,21 +4244,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D9CBEFE-8C4C-4054-8E02-CA457E93B4C8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>